<commit_message>
fixed issue 151: proposed data section displays empty fields if no data present (should be invisible)
</commit_message>
<xml_diff>
--- a/docs/design/CrossMdlAssign.xlsx
+++ b/docs/design/CrossMdlAssign.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1580" yWindow="0" windowWidth="25720" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="2580" yWindow="460" windowWidth="25720" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3254,108 +3254,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3424,12 +3322,6 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
@@ -3447,11 +3339,119 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="13" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="17" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="5" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="277">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -4063,8 +4063,8 @@
   <dimension ref="A1:AJ158"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G50" sqref="G50"/>
+      <pane ySplit="2" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4096,55 +4096,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" s="2" customFormat="1" ht="16" thickTop="1">
-      <c r="A1" s="188" t="s">
+      <c r="A1" s="251" t="s">
         <v>199</v>
       </c>
-      <c r="B1" s="188"/>
-      <c r="C1" s="189"/>
-      <c r="D1" s="160" t="s">
+      <c r="B1" s="251"/>
+      <c r="C1" s="252"/>
+      <c r="D1" s="257" t="s">
         <v>145</v>
       </c>
-      <c r="E1" s="161"/>
-      <c r="F1" s="162" t="s">
+      <c r="E1" s="258"/>
+      <c r="F1" s="259" t="s">
         <v>178</v>
       </c>
-      <c r="G1" s="161"/>
-      <c r="H1" s="162" t="s">
+      <c r="G1" s="258"/>
+      <c r="H1" s="259" t="s">
         <v>177</v>
       </c>
-      <c r="I1" s="161"/>
+      <c r="I1" s="258"/>
       <c r="J1" s="94" t="s">
         <v>172</v>
       </c>
-      <c r="K1" s="162" t="s">
+      <c r="K1" s="259" t="s">
         <v>203</v>
       </c>
-      <c r="L1" s="160"/>
+      <c r="L1" s="257"/>
       <c r="M1" s="90" t="s">
         <v>214</v>
       </c>
-      <c r="N1" s="158" t="s">
+      <c r="N1" s="255" t="s">
         <v>460</v>
       </c>
-      <c r="O1" s="156" t="s">
+      <c r="O1" s="253" t="s">
         <v>461</v>
       </c>
-      <c r="P1" s="184" t="s">
+      <c r="P1" s="247" t="s">
         <v>469</v>
       </c>
-      <c r="Q1" s="185"/>
-      <c r="R1" s="165" t="s">
+      <c r="Q1" s="248"/>
+      <c r="R1" s="225" t="s">
         <v>181</v>
       </c>
-      <c r="S1" s="166"/>
-      <c r="T1" s="181" t="s">
+      <c r="S1" s="226"/>
+      <c r="T1" s="242" t="s">
         <v>470</v>
       </c>
-      <c r="U1" s="182"/>
-      <c r="V1" s="181" t="s">
+      <c r="U1" s="243"/>
+      <c r="V1" s="242" t="s">
         <v>471</v>
       </c>
-      <c r="W1" s="182"/>
+      <c r="W1" s="243"/>
       <c r="X1" s="153" t="s">
         <v>472</v>
       </c>
@@ -4190,35 +4190,35 @@
       <c r="M2" s="137" t="s">
         <v>0</v>
       </c>
-      <c r="N2" s="159"/>
-      <c r="O2" s="157"/>
-      <c r="P2" s="186"/>
-      <c r="Q2" s="187"/>
-      <c r="R2" s="167"/>
-      <c r="S2" s="168"/>
+      <c r="N2" s="256"/>
+      <c r="O2" s="254"/>
+      <c r="P2" s="249"/>
+      <c r="Q2" s="250"/>
+      <c r="R2" s="227"/>
+      <c r="S2" s="228"/>
       <c r="T2" s="136" t="s">
         <v>0</v>
       </c>
       <c r="U2" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="V2" s="167"/>
-      <c r="W2" s="168"/>
+      <c r="V2" s="227"/>
+      <c r="W2" s="228"/>
       <c r="X2" s="154"/>
       <c r="Y2" s="47"/>
     </row>
     <row r="3" spans="1:25" s="39" customFormat="1" ht="16" thickTop="1">
-      <c r="A3" s="200" t="s">
+      <c r="A3" s="166" t="s">
         <v>297</v>
       </c>
-      <c r="B3" s="207" t="s">
+      <c r="B3" s="173" t="s">
         <v>298</v>
       </c>
-      <c r="C3" s="208"/>
-      <c r="D3" s="209" t="s">
+      <c r="C3" s="174"/>
+      <c r="D3" s="175" t="s">
         <v>517</v>
       </c>
-      <c r="E3" s="210" t="s">
+      <c r="E3" s="176" t="s">
         <v>531</v>
       </c>
       <c r="F3" s="68" t="s">
@@ -4241,24 +4241,24 @@
       <c r="S3" s="42"/>
       <c r="T3" s="10"/>
       <c r="U3" s="4"/>
-      <c r="V3" s="163" t="s">
+      <c r="V3" s="223" t="s">
         <v>506</v>
       </c>
-      <c r="W3" s="164"/>
+      <c r="W3" s="224"/>
       <c r="Y3" s="40"/>
     </row>
     <row r="4" spans="1:25" s="39" customFormat="1">
-      <c r="A4" s="200" t="s">
+      <c r="A4" s="166" t="s">
         <v>297</v>
       </c>
-      <c r="B4" s="207" t="s">
+      <c r="B4" s="173" t="s">
         <v>298</v>
       </c>
-      <c r="C4" s="208"/>
-      <c r="D4" s="209" t="s">
+      <c r="C4" s="174"/>
+      <c r="D4" s="175" t="s">
         <v>518</v>
       </c>
-      <c r="E4" s="210" t="s">
+      <c r="E4" s="176" t="s">
         <v>531</v>
       </c>
       <c r="F4" s="68" t="s">
@@ -4284,22 +4284,22 @@
       <c r="Y4" s="40"/>
     </row>
     <row r="5" spans="1:25" s="8" customFormat="1">
-      <c r="A5" s="192" t="s">
+      <c r="A5" s="158" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="193" t="s">
+      <c r="B5" s="159" t="s">
         <v>147</v>
       </c>
-      <c r="C5" s="194">
+      <c r="C5" s="160">
         <v>0</v>
       </c>
-      <c r="D5" s="195" t="s">
+      <c r="D5" s="161" t="s">
         <v>527</v>
       </c>
-      <c r="E5" s="197" t="s">
+      <c r="E5" s="163" t="s">
         <v>215</v>
       </c>
-      <c r="F5" s="195" t="s">
+      <c r="F5" s="161" t="s">
         <v>389</v>
       </c>
       <c r="G5" s="4"/>
@@ -4348,22 +4348,22 @@
       <c r="Y5" s="9"/>
     </row>
     <row r="6" spans="1:25" s="8" customFormat="1">
-      <c r="A6" s="192" t="s">
+      <c r="A6" s="158" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="193" t="s">
+      <c r="B6" s="159" t="s">
         <v>148</v>
       </c>
-      <c r="C6" s="194">
+      <c r="C6" s="160">
         <v>1</v>
       </c>
-      <c r="D6" s="195" t="s">
+      <c r="D6" s="161" t="s">
         <v>528</v>
       </c>
-      <c r="E6" s="197" t="s">
+      <c r="E6" s="163" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="193" t="s">
+      <c r="F6" s="159" t="s">
         <v>572</v>
       </c>
       <c r="G6" s="9" t="s">
@@ -4418,22 +4418,22 @@
       <c r="Y6" s="9"/>
     </row>
     <row r="7" spans="1:25" s="8" customFormat="1">
-      <c r="A7" s="192" t="s">
+      <c r="A7" s="158" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="193" t="s">
+      <c r="B7" s="159" t="s">
         <v>148</v>
       </c>
-      <c r="C7" s="194">
+      <c r="C7" s="160">
         <v>2</v>
       </c>
-      <c r="D7" s="195" t="s">
+      <c r="D7" s="161" t="s">
         <v>49</v>
       </c>
-      <c r="E7" s="197" t="s">
+      <c r="E7" s="163" t="s">
         <v>39</v>
       </c>
-      <c r="F7" s="193" t="s">
+      <c r="F7" s="159" t="s">
         <v>38</v>
       </c>
       <c r="G7" s="9" t="s">
@@ -4484,19 +4484,19 @@
       <c r="Y7" s="9"/>
     </row>
     <row r="8" spans="1:25" s="8" customFormat="1">
-      <c r="A8" s="192" t="s">
+      <c r="A8" s="158" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="193" t="s">
+      <c r="B8" s="159" t="s">
         <v>148</v>
       </c>
-      <c r="C8" s="194">
+      <c r="C8" s="160">
         <v>3</v>
       </c>
-      <c r="D8" s="195" t="s">
+      <c r="D8" s="161" t="s">
         <v>238</v>
       </c>
-      <c r="E8" s="196" t="s">
+      <c r="E8" s="162" t="s">
         <v>40</v>
       </c>
       <c r="F8" s="116" t="s">
@@ -4538,13 +4538,13 @@
       <c r="Y8" s="9"/>
     </row>
     <row r="9" spans="1:25">
-      <c r="A9" s="197"/>
-      <c r="B9" s="193"/>
-      <c r="C9" s="194"/>
-      <c r="D9" s="198" t="s">
+      <c r="A9" s="163"/>
+      <c r="B9" s="159"/>
+      <c r="C9" s="160"/>
+      <c r="D9" s="164" t="s">
         <v>41</v>
       </c>
-      <c r="E9" s="205" t="s">
+      <c r="E9" s="171" t="s">
         <v>42</v>
       </c>
       <c r="F9" s="5"/>
@@ -4569,11 +4569,11 @@
       <c r="W9" s="4"/>
     </row>
     <row r="10" spans="1:25">
-      <c r="A10" s="197"/>
-      <c r="B10" s="193"/>
-      <c r="C10" s="194"/>
-      <c r="D10" s="195"/>
-      <c r="E10" s="205" t="s">
+      <c r="A10" s="163"/>
+      <c r="B10" s="159"/>
+      <c r="C10" s="160"/>
+      <c r="D10" s="161"/>
+      <c r="E10" s="171" t="s">
         <v>43</v>
       </c>
       <c r="F10" s="5"/>
@@ -4602,11 +4602,11 @@
       <c r="W10" s="4"/>
     </row>
     <row r="11" spans="1:25">
-      <c r="A11" s="197"/>
-      <c r="B11" s="193"/>
-      <c r="C11" s="194"/>
-      <c r="D11" s="195"/>
-      <c r="E11" s="205" t="s">
+      <c r="A11" s="163"/>
+      <c r="B11" s="159"/>
+      <c r="C11" s="160"/>
+      <c r="D11" s="161"/>
+      <c r="E11" s="171" t="s">
         <v>44</v>
       </c>
       <c r="F11" s="5"/>
@@ -4633,11 +4633,11 @@
       <c r="W11" s="4"/>
     </row>
     <row r="12" spans="1:25" ht="16" thickBot="1">
-      <c r="A12" s="206"/>
-      <c r="B12" s="193"/>
-      <c r="C12" s="194"/>
-      <c r="D12" s="195"/>
-      <c r="E12" s="205" t="s">
+      <c r="A12" s="172"/>
+      <c r="B12" s="159"/>
+      <c r="C12" s="160"/>
+      <c r="D12" s="161"/>
+      <c r="E12" s="171" t="s">
         <v>174</v>
       </c>
       <c r="F12" s="5"/>
@@ -4666,15 +4666,15 @@
       <c r="W12" s="4"/>
     </row>
     <row r="13" spans="1:25">
-      <c r="A13" s="200" t="s">
+      <c r="A13" s="166" t="s">
         <v>297</v>
       </c>
-      <c r="B13" s="201"/>
-      <c r="C13" s="202"/>
-      <c r="D13" s="201" t="s">
+      <c r="B13" s="167"/>
+      <c r="C13" s="168"/>
+      <c r="D13" s="167" t="s">
         <v>508</v>
       </c>
-      <c r="E13" s="203" t="s">
+      <c r="E13" s="169" t="s">
         <v>513</v>
       </c>
       <c r="F13" s="5"/>
@@ -4697,15 +4697,15 @@
       <c r="W13" s="4"/>
     </row>
     <row r="14" spans="1:25">
-      <c r="A14" s="200" t="s">
+      <c r="A14" s="166" t="s">
         <v>297</v>
       </c>
-      <c r="B14" s="193"/>
-      <c r="C14" s="194"/>
-      <c r="D14" s="193" t="s">
+      <c r="B14" s="159"/>
+      <c r="C14" s="160"/>
+      <c r="D14" s="159" t="s">
         <v>510</v>
       </c>
-      <c r="E14" s="204" t="s">
+      <c r="E14" s="170" t="s">
         <v>514</v>
       </c>
       <c r="F14" s="5"/>
@@ -4728,15 +4728,15 @@
       <c r="W14" s="4"/>
     </row>
     <row r="15" spans="1:25">
-      <c r="A15" s="200" t="s">
+      <c r="A15" s="166" t="s">
         <v>297</v>
       </c>
-      <c r="B15" s="193"/>
-      <c r="C15" s="194"/>
-      <c r="D15" s="193" t="s">
+      <c r="B15" s="159"/>
+      <c r="C15" s="160"/>
+      <c r="D15" s="159" t="s">
         <v>524</v>
       </c>
-      <c r="E15" s="204" t="s">
+      <c r="E15" s="170" t="s">
         <v>525</v>
       </c>
       <c r="F15" s="5"/>
@@ -4759,18 +4759,18 @@
       <c r="W15" s="4"/>
     </row>
     <row r="16" spans="1:25">
-      <c r="A16" s="192"/>
-      <c r="B16" s="193" t="s">
+      <c r="A16" s="158"/>
+      <c r="B16" s="159" t="s">
         <v>148</v>
       </c>
-      <c r="C16" s="194"/>
-      <c r="D16" s="193" t="s">
+      <c r="C16" s="160"/>
+      <c r="D16" s="159" t="s">
         <v>49</v>
       </c>
-      <c r="E16" s="247" t="s">
+      <c r="E16" s="211" t="s">
         <v>509</v>
       </c>
-      <c r="F16" s="8"/>
+      <c r="F16" s="5"/>
       <c r="G16" s="4"/>
       <c r="H16" s="5"/>
       <c r="I16" s="4"/>
@@ -4790,15 +4790,15 @@
       <c r="W16" s="4"/>
     </row>
     <row r="17" spans="1:25">
-      <c r="A17" s="200" t="s">
+      <c r="A17" s="166" t="s">
         <v>297</v>
       </c>
-      <c r="B17" s="193"/>
-      <c r="C17" s="194"/>
-      <c r="D17" s="193" t="s">
+      <c r="B17" s="159"/>
+      <c r="C17" s="160"/>
+      <c r="D17" s="159" t="s">
         <v>511</v>
       </c>
-      <c r="E17" s="204" t="s">
+      <c r="E17" s="170" t="s">
         <v>515</v>
       </c>
       <c r="F17" s="5"/>
@@ -4821,15 +4821,15 @@
       <c r="W17" s="4"/>
     </row>
     <row r="18" spans="1:25">
-      <c r="A18" s="200" t="s">
+      <c r="A18" s="166" t="s">
         <v>297</v>
       </c>
-      <c r="B18" s="193"/>
-      <c r="C18" s="194"/>
-      <c r="D18" s="193" t="s">
+      <c r="B18" s="159"/>
+      <c r="C18" s="160"/>
+      <c r="D18" s="159" t="s">
         <v>512</v>
       </c>
-      <c r="E18" s="204" t="s">
+      <c r="E18" s="170" t="s">
         <v>516</v>
       </c>
       <c r="F18" s="5"/>
@@ -4852,15 +4852,15 @@
       <c r="W18" s="4"/>
     </row>
     <row r="19" spans="1:25">
-      <c r="A19" s="200" t="s">
+      <c r="A19" s="166" t="s">
         <v>297</v>
       </c>
-      <c r="B19" s="193"/>
-      <c r="C19" s="194"/>
-      <c r="D19" s="193" t="s">
+      <c r="B19" s="159"/>
+      <c r="C19" s="160"/>
+      <c r="D19" s="159" t="s">
         <v>526</v>
       </c>
-      <c r="E19" s="204" t="s">
+      <c r="E19" s="170" t="s">
         <v>525</v>
       </c>
       <c r="F19" s="5"/>
@@ -4883,18 +4883,18 @@
       <c r="W19" s="4"/>
     </row>
     <row r="20" spans="1:25" ht="16" thickBot="1">
-      <c r="A20" s="249"/>
-      <c r="B20" s="235" t="s">
+      <c r="A20" s="213"/>
+      <c r="B20" s="201" t="s">
         <v>148</v>
       </c>
-      <c r="C20" s="227"/>
-      <c r="D20" s="235" t="s">
+      <c r="C20" s="193"/>
+      <c r="D20" s="201" t="s">
         <v>49</v>
       </c>
-      <c r="E20" s="248" t="s">
+      <c r="E20" s="212" t="s">
         <v>219</v>
       </c>
-      <c r="F20" s="8"/>
+      <c r="F20" s="5"/>
       <c r="G20" s="4"/>
       <c r="H20" s="5"/>
       <c r="I20" s="4"/>
@@ -4914,13 +4914,13 @@
       <c r="W20" s="4"/>
     </row>
     <row r="21" spans="1:25">
-      <c r="A21" s="190" t="s">
+      <c r="A21" s="156" t="s">
         <v>6</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="C21" s="191">
+      <c r="C21" s="157">
         <v>4</v>
       </c>
       <c r="D21" s="8"/>
@@ -4959,13 +4959,13 @@
       <c r="W21" s="4"/>
     </row>
     <row r="22" spans="1:25">
-      <c r="A22" s="190" t="s">
+      <c r="A22" s="156" t="s">
         <v>7</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C22" s="191">
+      <c r="C22" s="157">
         <v>5</v>
       </c>
       <c r="D22" s="8"/>
@@ -5006,19 +5006,19 @@
       <c r="W22" s="4"/>
     </row>
     <row r="23" spans="1:25" s="8" customFormat="1">
-      <c r="A23" s="192" t="s">
+      <c r="A23" s="158" t="s">
         <v>8</v>
       </c>
-      <c r="B23" s="193" t="s">
+      <c r="B23" s="159" t="s">
         <v>148</v>
       </c>
-      <c r="C23" s="194">
+      <c r="C23" s="160">
         <v>6</v>
       </c>
-      <c r="D23" s="195" t="s">
+      <c r="D23" s="161" t="s">
         <v>49</v>
       </c>
-      <c r="E23" s="196" t="s">
+      <c r="E23" s="162" t="s">
         <v>53</v>
       </c>
       <c r="F23" s="31" t="s">
@@ -5060,13 +5060,13 @@
       <c r="Y23" s="9"/>
     </row>
     <row r="24" spans="1:25">
-      <c r="A24" s="197"/>
-      <c r="B24" s="193"/>
-      <c r="C24" s="194"/>
-      <c r="D24" s="198" t="s">
+      <c r="A24" s="163"/>
+      <c r="B24" s="159"/>
+      <c r="C24" s="160"/>
+      <c r="D24" s="164" t="s">
         <v>41</v>
       </c>
-      <c r="E24" s="199" t="s">
+      <c r="E24" s="165" t="s">
         <v>55</v>
       </c>
       <c r="F24" s="5"/>
@@ -5095,11 +5095,11 @@
       <c r="W24" s="4"/>
     </row>
     <row r="25" spans="1:25">
-      <c r="A25" s="197"/>
-      <c r="B25" s="193"/>
-      <c r="C25" s="194"/>
-      <c r="D25" s="195"/>
-      <c r="E25" s="199" t="s">
+      <c r="A25" s="163"/>
+      <c r="B25" s="159"/>
+      <c r="C25" s="160"/>
+      <c r="D25" s="161"/>
+      <c r="E25" s="165" t="s">
         <v>56</v>
       </c>
       <c r="F25" s="5"/>
@@ -5128,11 +5128,11 @@
       <c r="W25" s="4"/>
     </row>
     <row r="26" spans="1:25">
-      <c r="A26" s="197"/>
-      <c r="B26" s="193"/>
-      <c r="C26" s="194"/>
-      <c r="D26" s="195"/>
-      <c r="E26" s="199" t="s">
+      <c r="A26" s="163"/>
+      <c r="B26" s="159"/>
+      <c r="C26" s="160"/>
+      <c r="D26" s="161"/>
+      <c r="E26" s="165" t="s">
         <v>57</v>
       </c>
       <c r="F26" s="5"/>
@@ -5155,19 +5155,19 @@
       <c r="W26" s="4"/>
     </row>
     <row r="27" spans="1:25" s="8" customFormat="1">
-      <c r="A27" s="192" t="s">
+      <c r="A27" s="158" t="s">
         <v>9</v>
       </c>
-      <c r="B27" s="193" t="s">
+      <c r="B27" s="159" t="s">
         <v>147</v>
       </c>
-      <c r="C27" s="194">
+      <c r="C27" s="160">
         <v>7</v>
       </c>
-      <c r="D27" s="195" t="s">
+      <c r="D27" s="161" t="s">
         <v>529</v>
       </c>
-      <c r="E27" s="197" t="s">
+      <c r="E27" s="163" t="s">
         <v>58</v>
       </c>
       <c r="F27" s="31" t="s">
@@ -5211,19 +5211,19 @@
       <c r="Y27" s="9"/>
     </row>
     <row r="28" spans="1:25" s="8" customFormat="1">
-      <c r="A28" s="192" t="s">
+      <c r="A28" s="158" t="s">
         <v>10</v>
       </c>
-      <c r="B28" s="193" t="s">
+      <c r="B28" s="159" t="s">
         <v>147</v>
       </c>
-      <c r="C28" s="194">
+      <c r="C28" s="160">
         <v>8</v>
       </c>
-      <c r="D28" s="195" t="s">
+      <c r="D28" s="161" t="s">
         <v>530</v>
       </c>
-      <c r="E28" s="197" t="s">
+      <c r="E28" s="163" t="s">
         <v>59</v>
       </c>
       <c r="F28" s="31" t="s">
@@ -5267,19 +5267,19 @@
       <c r="Y28" s="9"/>
     </row>
     <row r="29" spans="1:25" s="8" customFormat="1">
-      <c r="A29" s="192" t="s">
+      <c r="A29" s="158" t="s">
         <v>11</v>
       </c>
-      <c r="B29" s="193" t="s">
+      <c r="B29" s="159" t="s">
         <v>148</v>
       </c>
-      <c r="C29" s="194">
+      <c r="C29" s="160">
         <v>9</v>
       </c>
-      <c r="D29" s="195" t="s">
+      <c r="D29" s="161" t="s">
         <v>49</v>
       </c>
-      <c r="E29" s="196" t="s">
+      <c r="E29" s="162" t="s">
         <v>60</v>
       </c>
       <c r="F29" s="32" t="s">
@@ -5323,13 +5323,13 @@
       <c r="Y29" s="9"/>
     </row>
     <row r="30" spans="1:25">
-      <c r="A30" s="197"/>
-      <c r="B30" s="193"/>
-      <c r="C30" s="194"/>
-      <c r="D30" s="198" t="s">
+      <c r="A30" s="163"/>
+      <c r="B30" s="159"/>
+      <c r="C30" s="160"/>
+      <c r="D30" s="164" t="s">
         <v>41</v>
       </c>
-      <c r="E30" s="199" t="s">
+      <c r="E30" s="165" t="s">
         <v>61</v>
       </c>
       <c r="F30" s="5"/>
@@ -5352,11 +5352,11 @@
       <c r="W30" s="4"/>
     </row>
     <row r="31" spans="1:25">
-      <c r="A31" s="197"/>
-      <c r="B31" s="193"/>
-      <c r="C31" s="194"/>
-      <c r="D31" s="195"/>
-      <c r="E31" s="199" t="s">
+      <c r="A31" s="163"/>
+      <c r="B31" s="159"/>
+      <c r="C31" s="160"/>
+      <c r="D31" s="161"/>
+      <c r="E31" s="165" t="s">
         <v>64</v>
       </c>
       <c r="F31" s="5"/>
@@ -5379,11 +5379,11 @@
       <c r="W31" s="4"/>
     </row>
     <row r="32" spans="1:25">
-      <c r="A32" s="197"/>
-      <c r="B32" s="193"/>
-      <c r="C32" s="194"/>
-      <c r="D32" s="195"/>
-      <c r="E32" s="199" t="s">
+      <c r="A32" s="163"/>
+      <c r="B32" s="159"/>
+      <c r="C32" s="160"/>
+      <c r="D32" s="161"/>
+      <c r="E32" s="165" t="s">
         <v>62</v>
       </c>
       <c r="F32" s="5"/>
@@ -5406,11 +5406,11 @@
       <c r="W32" s="4"/>
     </row>
     <row r="33" spans="1:25">
-      <c r="A33" s="197"/>
-      <c r="B33" s="193"/>
-      <c r="C33" s="194"/>
-      <c r="D33" s="195"/>
-      <c r="E33" s="199" t="s">
+      <c r="A33" s="163"/>
+      <c r="B33" s="159"/>
+      <c r="C33" s="160"/>
+      <c r="D33" s="161"/>
+      <c r="E33" s="165" t="s">
         <v>63</v>
       </c>
       <c r="F33" s="5"/>
@@ -5433,11 +5433,11 @@
       <c r="W33" s="4"/>
     </row>
     <row r="34" spans="1:25">
-      <c r="A34" s="197"/>
-      <c r="B34" s="193"/>
-      <c r="C34" s="194"/>
-      <c r="D34" s="195"/>
-      <c r="E34" s="199" t="s">
+      <c r="A34" s="163"/>
+      <c r="B34" s="159"/>
+      <c r="C34" s="160"/>
+      <c r="D34" s="161"/>
+      <c r="E34" s="165" t="s">
         <v>65</v>
       </c>
       <c r="F34" s="5"/>
@@ -5460,19 +5460,19 @@
       <c r="W34" s="4"/>
     </row>
     <row r="35" spans="1:25" s="8" customFormat="1">
-      <c r="A35" s="192" t="s">
+      <c r="A35" s="158" t="s">
         <v>12</v>
       </c>
-      <c r="B35" s="193" t="s">
+      <c r="B35" s="159" t="s">
         <v>148</v>
       </c>
-      <c r="C35" s="194">
+      <c r="C35" s="160">
         <v>10</v>
       </c>
-      <c r="D35" s="195" t="s">
+      <c r="D35" s="161" t="s">
         <v>532</v>
       </c>
-      <c r="E35" s="197" t="s">
+      <c r="E35" s="163" t="s">
         <v>66</v>
       </c>
       <c r="F35" s="32" t="s">
@@ -5514,19 +5514,19 @@
       <c r="Y35" s="9"/>
     </row>
     <row r="36" spans="1:25" s="8" customFormat="1">
-      <c r="A36" s="192" t="s">
+      <c r="A36" s="158" t="s">
         <v>13</v>
       </c>
-      <c r="B36" s="193" t="s">
+      <c r="B36" s="159" t="s">
         <v>148</v>
       </c>
-      <c r="C36" s="194">
+      <c r="C36" s="160">
         <v>11</v>
       </c>
-      <c r="D36" s="195" t="s">
+      <c r="D36" s="161" t="s">
         <v>533</v>
       </c>
-      <c r="E36" s="197" t="s">
+      <c r="E36" s="163" t="s">
         <v>67</v>
       </c>
       <c r="F36" s="32" t="s">
@@ -5570,19 +5570,19 @@
       <c r="Y36" s="9"/>
     </row>
     <row r="37" spans="1:25" s="8" customFormat="1">
-      <c r="A37" s="192" t="s">
+      <c r="A37" s="158" t="s">
         <v>14</v>
       </c>
-      <c r="B37" s="193" t="s">
+      <c r="B37" s="159" t="s">
         <v>148</v>
       </c>
-      <c r="C37" s="194">
+      <c r="C37" s="160">
         <v>12</v>
       </c>
-      <c r="D37" s="195" t="s">
+      <c r="D37" s="161" t="s">
         <v>534</v>
       </c>
-      <c r="E37" s="197" t="s">
+      <c r="E37" s="163" t="s">
         <v>68</v>
       </c>
       <c r="F37" s="32" t="s">
@@ -5624,19 +5624,19 @@
       <c r="Y37" s="9"/>
     </row>
     <row r="38" spans="1:25" s="8" customFormat="1">
-      <c r="A38" s="192" t="s">
+      <c r="A38" s="158" t="s">
         <v>15</v>
       </c>
-      <c r="B38" s="193" t="s">
+      <c r="B38" s="159" t="s">
         <v>148</v>
       </c>
-      <c r="C38" s="194">
+      <c r="C38" s="160">
         <v>13</v>
       </c>
-      <c r="D38" s="195" t="s">
+      <c r="D38" s="161" t="s">
         <v>238</v>
       </c>
-      <c r="E38" s="197" t="s">
+      <c r="E38" s="163" t="s">
         <v>92</v>
       </c>
       <c r="F38" s="32" t="s">
@@ -5680,13 +5680,13 @@
       <c r="Y38" s="9"/>
     </row>
     <row r="39" spans="1:25">
-      <c r="A39" s="197"/>
-      <c r="B39" s="193"/>
-      <c r="C39" s="194"/>
-      <c r="D39" s="198" t="s">
+      <c r="A39" s="163"/>
+      <c r="B39" s="159"/>
+      <c r="C39" s="160"/>
+      <c r="D39" s="164" t="s">
         <v>41</v>
       </c>
-      <c r="E39" s="199" t="s">
+      <c r="E39" s="165" t="s">
         <v>93</v>
       </c>
       <c r="F39" s="5"/>
@@ -5709,11 +5709,11 @@
       <c r="W39" s="4"/>
     </row>
     <row r="40" spans="1:25">
-      <c r="A40" s="197"/>
-      <c r="B40" s="193"/>
-      <c r="C40" s="194"/>
-      <c r="D40" s="195"/>
-      <c r="E40" s="199" t="s">
+      <c r="A40" s="163"/>
+      <c r="B40" s="159"/>
+      <c r="C40" s="160"/>
+      <c r="D40" s="161"/>
+      <c r="E40" s="165" t="s">
         <v>94</v>
       </c>
       <c r="F40" s="5"/>
@@ -5735,49 +5735,49 @@
       <c r="V40" s="5"/>
       <c r="W40" s="4"/>
     </row>
-    <row r="41" spans="1:25" s="223" customFormat="1">
-      <c r="A41" s="214"/>
-      <c r="B41" s="215"/>
-      <c r="C41" s="216"/>
-      <c r="D41" s="215"/>
-      <c r="E41" s="217" t="s">
+    <row r="41" spans="1:25" s="189" customFormat="1">
+      <c r="A41" s="180"/>
+      <c r="B41" s="181"/>
+      <c r="C41" s="182"/>
+      <c r="D41" s="181"/>
+      <c r="E41" s="183" t="s">
         <v>95</v>
       </c>
-      <c r="F41" s="218"/>
-      <c r="G41" s="219"/>
-      <c r="H41" s="218"/>
-      <c r="I41" s="219"/>
-      <c r="J41" s="220"/>
-      <c r="K41" s="221"/>
-      <c r="L41" s="222"/>
-      <c r="M41" s="222"/>
-      <c r="N41" s="219"/>
-      <c r="O41" s="219"/>
-      <c r="P41" s="218"/>
-      <c r="Q41" s="219"/>
-      <c r="R41" s="218"/>
-      <c r="S41" s="219"/>
-      <c r="T41" s="218"/>
-      <c r="U41" s="219"/>
-      <c r="V41" s="218"/>
-      <c r="W41" s="219"/>
-      <c r="Y41" s="224"/>
+      <c r="F41" s="184"/>
+      <c r="G41" s="185"/>
+      <c r="H41" s="184"/>
+      <c r="I41" s="185"/>
+      <c r="J41" s="186"/>
+      <c r="K41" s="187"/>
+      <c r="L41" s="188"/>
+      <c r="M41" s="188"/>
+      <c r="N41" s="185"/>
+      <c r="O41" s="185"/>
+      <c r="P41" s="184"/>
+      <c r="Q41" s="185"/>
+      <c r="R41" s="184"/>
+      <c r="S41" s="185"/>
+      <c r="T41" s="184"/>
+      <c r="U41" s="185"/>
+      <c r="V41" s="184"/>
+      <c r="W41" s="185"/>
+      <c r="Y41" s="190"/>
     </row>
     <row r="42" spans="1:25" s="8" customFormat="1">
-      <c r="A42" s="211" t="s">
+      <c r="A42" s="177" t="s">
         <v>297</v>
       </c>
-      <c r="B42" s="212" t="s">
+      <c r="B42" s="178" t="s">
         <v>300</v>
       </c>
-      <c r="C42" s="194"/>
-      <c r="D42" s="213" t="s">
+      <c r="C42" s="160"/>
+      <c r="D42" s="179" t="s">
         <v>535</v>
       </c>
-      <c r="E42" s="197" t="s">
+      <c r="E42" s="163" t="s">
         <v>299</v>
       </c>
-      <c r="F42" s="259" t="s">
+      <c r="F42" s="222" t="s">
         <v>322</v>
       </c>
       <c r="G42" s="53" t="s">
@@ -5808,18 +5808,18 @@
       <c r="Y42" s="9"/>
     </row>
     <row r="43" spans="1:25" s="8" customFormat="1">
-      <c r="A43" s="211" t="s">
+      <c r="A43" s="177" t="s">
         <v>577</v>
       </c>
-      <c r="B43" s="212"/>
-      <c r="C43" s="194"/>
-      <c r="D43" s="213" t="s">
+      <c r="B43" s="178"/>
+      <c r="C43" s="160"/>
+      <c r="D43" s="179" t="s">
         <v>539</v>
       </c>
-      <c r="E43" s="197" t="s">
+      <c r="E43" s="163" t="s">
         <v>303</v>
       </c>
-      <c r="F43" s="259" t="s">
+      <c r="F43" s="222" t="s">
         <v>579</v>
       </c>
       <c r="G43" s="53"/>
@@ -5842,20 +5842,20 @@
       <c r="Y43" s="9"/>
     </row>
     <row r="44" spans="1:25" s="8" customFormat="1">
-      <c r="A44" s="211" t="s">
+      <c r="A44" s="177" t="s">
         <v>297</v>
       </c>
-      <c r="B44" s="212" t="s">
+      <c r="B44" s="178" t="s">
         <v>302</v>
       </c>
-      <c r="C44" s="194"/>
-      <c r="D44" s="213" t="s">
+      <c r="C44" s="160"/>
+      <c r="D44" s="179" t="s">
         <v>536</v>
       </c>
-      <c r="E44" s="197" t="s">
+      <c r="E44" s="163" t="s">
         <v>301</v>
       </c>
-      <c r="F44" s="259" t="s">
+      <c r="F44" s="222" t="s">
         <v>575</v>
       </c>
       <c r="G44" s="38"/>
@@ -5878,15 +5878,15 @@
       <c r="Y44" s="9"/>
     </row>
     <row r="45" spans="1:25" s="8" customFormat="1">
-      <c r="A45" s="211" t="s">
+      <c r="A45" s="177" t="s">
         <v>297</v>
       </c>
-      <c r="B45" s="212"/>
-      <c r="C45" s="194"/>
-      <c r="D45" s="198" t="s">
+      <c r="B45" s="178"/>
+      <c r="C45" s="160"/>
+      <c r="D45" s="164" t="s">
         <v>41</v>
       </c>
-      <c r="E45" s="199" t="s">
+      <c r="E45" s="165" t="s">
         <v>521</v>
       </c>
       <c r="F45" s="37"/>
@@ -5910,11 +5910,11 @@
       <c r="Y45" s="9"/>
     </row>
     <row r="46" spans="1:25" s="8" customFormat="1">
-      <c r="A46" s="211"/>
-      <c r="B46" s="212"/>
-      <c r="C46" s="194"/>
-      <c r="D46" s="213"/>
-      <c r="E46" s="199" t="s">
+      <c r="A46" s="177"/>
+      <c r="B46" s="178"/>
+      <c r="C46" s="160"/>
+      <c r="D46" s="179"/>
+      <c r="E46" s="165" t="s">
         <v>522</v>
       </c>
       <c r="F46" s="37"/>
@@ -5938,11 +5938,11 @@
       <c r="Y46" s="9"/>
     </row>
     <row r="47" spans="1:25" s="8" customFormat="1">
-      <c r="A47" s="211"/>
-      <c r="B47" s="212"/>
-      <c r="C47" s="194"/>
-      <c r="D47" s="213"/>
-      <c r="E47" s="199" t="s">
+      <c r="A47" s="177"/>
+      <c r="B47" s="178"/>
+      <c r="C47" s="160"/>
+      <c r="D47" s="179"/>
+      <c r="E47" s="165" t="s">
         <v>523</v>
       </c>
       <c r="F47" s="37"/>
@@ -5966,18 +5966,18 @@
       <c r="Y47" s="9"/>
     </row>
     <row r="48" spans="1:25" s="8" customFormat="1">
-      <c r="A48" s="211" t="s">
+      <c r="A48" s="177" t="s">
         <v>578</v>
       </c>
-      <c r="B48" s="212"/>
-      <c r="C48" s="194"/>
-      <c r="D48" s="213" t="s">
+      <c r="B48" s="178"/>
+      <c r="C48" s="160"/>
+      <c r="D48" s="179" t="s">
         <v>540</v>
       </c>
-      <c r="E48" s="197" t="s">
+      <c r="E48" s="163" t="s">
         <v>303</v>
       </c>
-      <c r="F48" s="259" t="s">
+      <c r="F48" s="222" t="s">
         <v>580</v>
       </c>
       <c r="G48" s="38"/>
@@ -6000,20 +6000,20 @@
       <c r="Y48" s="9"/>
     </row>
     <row r="49" spans="1:25" s="8" customFormat="1">
-      <c r="A49" s="211" t="s">
+      <c r="A49" s="177" t="s">
         <v>297</v>
       </c>
-      <c r="B49" s="212" t="s">
+      <c r="B49" s="178" t="s">
         <v>302</v>
       </c>
-      <c r="C49" s="194"/>
-      <c r="D49" s="213" t="s">
+      <c r="C49" s="160"/>
+      <c r="D49" s="179" t="s">
         <v>537</v>
       </c>
-      <c r="E49" s="197" t="s">
+      <c r="E49" s="163" t="s">
         <v>301</v>
       </c>
-      <c r="F49" s="259" t="s">
+      <c r="F49" s="222" t="s">
         <v>575</v>
       </c>
       <c r="G49" s="38"/>
@@ -6036,13 +6036,13 @@
       <c r="Y49" s="9"/>
     </row>
     <row r="50" spans="1:25" s="8" customFormat="1">
-      <c r="A50" s="211"/>
-      <c r="B50" s="212"/>
-      <c r="C50" s="194"/>
-      <c r="D50" s="198" t="s">
+      <c r="A50" s="177"/>
+      <c r="B50" s="178"/>
+      <c r="C50" s="160"/>
+      <c r="D50" s="164" t="s">
         <v>41</v>
       </c>
-      <c r="E50" s="199" t="s">
+      <c r="E50" s="165" t="s">
         <v>521</v>
       </c>
       <c r="F50" s="37"/>
@@ -6066,11 +6066,11 @@
       <c r="Y50" s="9"/>
     </row>
     <row r="51" spans="1:25" s="8" customFormat="1">
-      <c r="A51" s="211"/>
-      <c r="B51" s="212"/>
-      <c r="C51" s="194"/>
-      <c r="D51" s="213"/>
-      <c r="E51" s="199" t="s">
+      <c r="A51" s="177"/>
+      <c r="B51" s="178"/>
+      <c r="C51" s="160"/>
+      <c r="D51" s="179"/>
+      <c r="E51" s="165" t="s">
         <v>522</v>
       </c>
       <c r="F51" s="37"/>
@@ -6094,11 +6094,11 @@
       <c r="Y51" s="9"/>
     </row>
     <row r="52" spans="1:25" s="8" customFormat="1">
-      <c r="A52" s="211"/>
-      <c r="B52" s="212"/>
-      <c r="C52" s="194"/>
-      <c r="D52" s="213"/>
-      <c r="E52" s="199" t="s">
+      <c r="A52" s="177"/>
+      <c r="B52" s="178"/>
+      <c r="C52" s="160"/>
+      <c r="D52" s="179"/>
+      <c r="E52" s="165" t="s">
         <v>523</v>
       </c>
       <c r="F52" s="37"/>
@@ -6122,18 +6122,18 @@
       <c r="Y52" s="9"/>
     </row>
     <row r="53" spans="1:25" s="8" customFormat="1">
-      <c r="A53" s="211" t="s">
+      <c r="A53" s="177" t="s">
         <v>576</v>
       </c>
-      <c r="B53" s="212"/>
-      <c r="C53" s="194"/>
-      <c r="D53" s="213" t="s">
+      <c r="B53" s="178"/>
+      <c r="C53" s="160"/>
+      <c r="D53" s="179" t="s">
         <v>541</v>
       </c>
-      <c r="E53" s="197" t="s">
+      <c r="E53" s="163" t="s">
         <v>303</v>
       </c>
-      <c r="F53" s="259" t="s">
+      <c r="F53" s="222" t="s">
         <v>581</v>
       </c>
       <c r="G53" s="38"/>
@@ -6156,20 +6156,20 @@
       <c r="Y53" s="9"/>
     </row>
     <row r="54" spans="1:25" s="8" customFormat="1">
-      <c r="A54" s="211" t="s">
+      <c r="A54" s="177" t="s">
         <v>297</v>
       </c>
-      <c r="B54" s="212" t="s">
+      <c r="B54" s="178" t="s">
         <v>302</v>
       </c>
-      <c r="C54" s="194"/>
-      <c r="D54" s="213" t="s">
+      <c r="C54" s="160"/>
+      <c r="D54" s="179" t="s">
         <v>538</v>
       </c>
-      <c r="E54" s="197" t="s">
+      <c r="E54" s="163" t="s">
         <v>301</v>
       </c>
-      <c r="F54" s="259" t="s">
+      <c r="F54" s="222" t="s">
         <v>575</v>
       </c>
       <c r="G54" s="38"/>
@@ -6192,13 +6192,13 @@
       <c r="Y54" s="9"/>
     </row>
     <row r="55" spans="1:25" s="8" customFormat="1">
-      <c r="A55" s="211"/>
-      <c r="B55" s="212"/>
-      <c r="C55" s="194"/>
-      <c r="D55" s="198" t="s">
+      <c r="A55" s="177"/>
+      <c r="B55" s="178"/>
+      <c r="C55" s="160"/>
+      <c r="D55" s="164" t="s">
         <v>41</v>
       </c>
-      <c r="E55" s="199" t="s">
+      <c r="E55" s="165" t="s">
         <v>521</v>
       </c>
       <c r="F55" s="37"/>
@@ -6222,11 +6222,11 @@
       <c r="Y55" s="9"/>
     </row>
     <row r="56" spans="1:25" s="8" customFormat="1">
-      <c r="A56" s="211"/>
-      <c r="B56" s="212"/>
-      <c r="C56" s="194"/>
-      <c r="D56" s="213"/>
-      <c r="E56" s="199" t="s">
+      <c r="A56" s="177"/>
+      <c r="B56" s="178"/>
+      <c r="C56" s="160"/>
+      <c r="D56" s="179"/>
+      <c r="E56" s="165" t="s">
         <v>522</v>
       </c>
       <c r="F56" s="37"/>
@@ -6250,11 +6250,11 @@
       <c r="Y56" s="9"/>
     </row>
     <row r="57" spans="1:25" s="8" customFormat="1">
-      <c r="A57" s="211"/>
-      <c r="B57" s="212"/>
-      <c r="C57" s="194"/>
-      <c r="D57" s="213"/>
-      <c r="E57" s="199" t="s">
+      <c r="A57" s="177"/>
+      <c r="B57" s="178"/>
+      <c r="C57" s="160"/>
+      <c r="D57" s="179"/>
+      <c r="E57" s="165" t="s">
         <v>523</v>
       </c>
       <c r="F57" s="37"/>
@@ -6278,14 +6278,14 @@
       <c r="Y57" s="9"/>
     </row>
     <row r="58" spans="1:25" s="8" customFormat="1">
-      <c r="A58" s="211" t="s">
+      <c r="A58" s="177" t="s">
         <v>297</v>
       </c>
-      <c r="B58" s="212" t="s">
+      <c r="B58" s="178" t="s">
         <v>304</v>
       </c>
-      <c r="C58" s="194"/>
-      <c r="D58" s="213" t="s">
+      <c r="C58" s="160"/>
+      <c r="D58" s="179" t="s">
         <v>539</v>
       </c>
       <c r="E58" s="117" t="s">
@@ -6314,14 +6314,14 @@
       <c r="Y58" s="9"/>
     </row>
     <row r="59" spans="1:25" s="8" customFormat="1">
-      <c r="A59" s="211" t="s">
+      <c r="A59" s="177" t="s">
         <v>297</v>
       </c>
-      <c r="B59" s="212" t="s">
+      <c r="B59" s="178" t="s">
         <v>304</v>
       </c>
-      <c r="C59" s="194"/>
-      <c r="D59" s="213" t="s">
+      <c r="C59" s="160"/>
+      <c r="D59" s="179" t="s">
         <v>540</v>
       </c>
       <c r="E59" s="117" t="s">
@@ -6350,14 +6350,14 @@
       <c r="Y59" s="9"/>
     </row>
     <row r="60" spans="1:25" s="8" customFormat="1">
-      <c r="A60" s="211" t="s">
+      <c r="A60" s="177" t="s">
         <v>297</v>
       </c>
-      <c r="B60" s="212" t="s">
+      <c r="B60" s="178" t="s">
         <v>304</v>
       </c>
-      <c r="C60" s="194"/>
-      <c r="D60" s="213" t="s">
+      <c r="C60" s="160"/>
+      <c r="D60" s="179" t="s">
         <v>541</v>
       </c>
       <c r="E60" s="117" t="s">
@@ -6386,14 +6386,14 @@
       <c r="Y60" s="9"/>
     </row>
     <row r="61" spans="1:25" s="8" customFormat="1">
-      <c r="A61" s="211" t="s">
+      <c r="A61" s="177" t="s">
         <v>297</v>
       </c>
-      <c r="B61" s="212" t="s">
+      <c r="B61" s="178" t="s">
         <v>302</v>
       </c>
-      <c r="C61" s="194"/>
-      <c r="D61" s="213" t="s">
+      <c r="C61" s="160"/>
+      <c r="D61" s="179" t="s">
         <v>542</v>
       </c>
       <c r="E61" s="117" t="s">
@@ -6424,11 +6424,11 @@
       <c r="Y61" s="9"/>
     </row>
     <row r="62" spans="1:25" s="16" customFormat="1" ht="16" thickBot="1">
-      <c r="A62" s="225"/>
-      <c r="B62" s="226"/>
-      <c r="C62" s="227"/>
-      <c r="D62" s="228"/>
-      <c r="E62" s="229"/>
+      <c r="A62" s="191"/>
+      <c r="B62" s="192"/>
+      <c r="C62" s="193"/>
+      <c r="D62" s="194"/>
+      <c r="E62" s="195"/>
       <c r="F62" s="73" t="s">
         <v>334</v>
       </c>
@@ -6610,17 +6610,17 @@
       <c r="Y67" s="18"/>
     </row>
     <row r="68" spans="1:36" s="8" customFormat="1">
-      <c r="A68" s="230" t="s">
+      <c r="A68" s="196" t="s">
         <v>104</v>
       </c>
-      <c r="B68" s="231"/>
-      <c r="C68" s="194">
+      <c r="B68" s="197"/>
+      <c r="C68" s="160">
         <v>17</v>
       </c>
-      <c r="D68" s="195" t="s">
+      <c r="D68" s="161" t="s">
         <v>99</v>
       </c>
-      <c r="E68" s="232" t="s">
+      <c r="E68" s="198" t="s">
         <v>103</v>
       </c>
       <c r="F68" s="31" t="s">
@@ -6658,13 +6658,13 @@
       <c r="Y68" s="9"/>
     </row>
     <row r="69" spans="1:36" s="16" customFormat="1" ht="16" thickBot="1">
-      <c r="A69" s="233" t="s">
+      <c r="A69" s="199" t="s">
         <v>543</v>
       </c>
-      <c r="B69" s="234"/>
-      <c r="C69" s="227"/>
-      <c r="D69" s="235"/>
-      <c r="E69" s="236"/>
+      <c r="B69" s="200"/>
+      <c r="C69" s="193"/>
+      <c r="D69" s="201"/>
+      <c r="E69" s="202"/>
       <c r="F69" s="83" t="s">
         <v>237</v>
       </c>
@@ -6918,17 +6918,17 @@
       <c r="Y75" s="15"/>
     </row>
     <row r="76" spans="1:36">
-      <c r="A76" s="230" t="s">
+      <c r="A76" s="196" t="s">
         <v>221</v>
       </c>
-      <c r="B76" s="193"/>
-      <c r="C76" s="194" t="s">
+      <c r="B76" s="159"/>
+      <c r="C76" s="160" t="s">
         <v>293</v>
       </c>
-      <c r="D76" s="195" t="s">
+      <c r="D76" s="161" t="s">
         <v>99</v>
       </c>
-      <c r="E76" s="232" t="s">
+      <c r="E76" s="198" t="s">
         <v>120</v>
       </c>
       <c r="F76" s="31" t="s">
@@ -6967,13 +6967,13 @@
       <c r="W76" s="4"/>
     </row>
     <row r="77" spans="1:36">
-      <c r="A77" s="240" t="s">
+      <c r="A77" s="204" t="s">
         <v>245</v>
       </c>
-      <c r="B77" s="193"/>
-      <c r="C77" s="194"/>
-      <c r="D77" s="195"/>
-      <c r="E77" s="232"/>
+      <c r="B77" s="159"/>
+      <c r="C77" s="160"/>
+      <c r="D77" s="161"/>
+      <c r="E77" s="198"/>
       <c r="F77" s="51" t="s">
         <v>237</v>
       </c>
@@ -7086,17 +7086,17 @@
       <c r="W79" s="18"/>
     </row>
     <row r="80" spans="1:36">
-      <c r="A80" s="230" t="s">
+      <c r="A80" s="196" t="s">
         <v>222</v>
       </c>
-      <c r="B80" s="193"/>
-      <c r="C80" s="194" t="s">
+      <c r="B80" s="159"/>
+      <c r="C80" s="160" t="s">
         <v>294</v>
       </c>
-      <c r="D80" s="195" t="s">
+      <c r="D80" s="161" t="s">
         <v>99</v>
       </c>
-      <c r="E80" s="232" t="s">
+      <c r="E80" s="198" t="s">
         <v>121</v>
       </c>
       <c r="F80" s="31" t="s">
@@ -7142,13 +7142,13 @@
       <c r="AJ80" s="6"/>
     </row>
     <row r="81" spans="1:36">
-      <c r="A81" s="240" t="s">
+      <c r="A81" s="204" t="s">
         <v>245</v>
       </c>
-      <c r="B81" s="193"/>
-      <c r="C81" s="194"/>
-      <c r="D81" s="195"/>
-      <c r="E81" s="232"/>
+      <c r="B81" s="159"/>
+      <c r="C81" s="160"/>
+      <c r="D81" s="161"/>
+      <c r="E81" s="198"/>
       <c r="F81" s="51" t="s">
         <v>237</v>
       </c>
@@ -7269,17 +7269,17 @@
       <c r="W83" s="18"/>
     </row>
     <row r="84" spans="1:36">
-      <c r="A84" s="237" t="s">
+      <c r="A84" s="203" t="s">
         <v>227</v>
       </c>
-      <c r="B84" s="238" t="s">
+      <c r="B84" s="245" t="s">
         <v>239</v>
       </c>
-      <c r="C84" s="239"/>
-      <c r="D84" s="195" t="s">
+      <c r="C84" s="246"/>
+      <c r="D84" s="161" t="s">
         <v>99</v>
       </c>
-      <c r="E84" s="232" t="s">
+      <c r="E84" s="198" t="s">
         <v>223</v>
       </c>
       <c r="F84" s="49" t="s">
@@ -7325,15 +7325,15 @@
       <c r="AJ84" s="6"/>
     </row>
     <row r="85" spans="1:36">
-      <c r="A85" s="240" t="s">
+      <c r="A85" s="204" t="s">
         <v>245</v>
       </c>
-      <c r="B85" s="193"/>
-      <c r="C85" s="194"/>
-      <c r="D85" s="195" t="s">
+      <c r="B85" s="159"/>
+      <c r="C85" s="160"/>
+      <c r="D85" s="161" t="s">
         <v>49</v>
       </c>
-      <c r="E85" s="197" t="s">
+      <c r="E85" s="163" t="s">
         <v>233</v>
       </c>
       <c r="F85" s="51" t="s">
@@ -7360,13 +7360,13 @@
       <c r="W85" s="4"/>
     </row>
     <row r="86" spans="1:36">
-      <c r="A86" s="230"/>
-      <c r="B86" s="193"/>
-      <c r="C86" s="194"/>
-      <c r="D86" s="198" t="s">
+      <c r="A86" s="196"/>
+      <c r="B86" s="159"/>
+      <c r="C86" s="160"/>
+      <c r="D86" s="164" t="s">
         <v>41</v>
       </c>
-      <c r="E86" s="241" t="s">
+      <c r="E86" s="205" t="s">
         <v>231</v>
       </c>
       <c r="F86" s="54" t="s">
@@ -7399,11 +7399,11 @@
       <c r="W86" s="4"/>
     </row>
     <row r="87" spans="1:36" s="24" customFormat="1" ht="16" thickBot="1">
-      <c r="A87" s="242"/>
-      <c r="B87" s="235"/>
-      <c r="C87" s="227"/>
-      <c r="D87" s="235"/>
-      <c r="E87" s="243" t="s">
+      <c r="A87" s="206"/>
+      <c r="B87" s="201"/>
+      <c r="C87" s="193"/>
+      <c r="D87" s="201"/>
+      <c r="E87" s="207" t="s">
         <v>232</v>
       </c>
       <c r="F87" s="73" t="s">
@@ -7437,17 +7437,17 @@
       <c r="Y87" s="25"/>
     </row>
     <row r="88" spans="1:36">
-      <c r="A88" s="237" t="s">
+      <c r="A88" s="203" t="s">
         <v>228</v>
       </c>
-      <c r="B88" s="238" t="s">
+      <c r="B88" s="245" t="s">
         <v>239</v>
       </c>
-      <c r="C88" s="239"/>
-      <c r="D88" s="244" t="s">
+      <c r="C88" s="246"/>
+      <c r="D88" s="208" t="s">
         <v>99</v>
       </c>
-      <c r="E88" s="232" t="s">
+      <c r="E88" s="198" t="s">
         <v>224</v>
       </c>
       <c r="F88" s="32" t="s">
@@ -7480,12 +7480,12 @@
       <c r="W88" s="4"/>
     </row>
     <row r="89" spans="1:36">
-      <c r="A89" s="240" t="s">
+      <c r="A89" s="204" t="s">
         <v>245</v>
       </c>
-      <c r="B89" s="193"/>
-      <c r="C89" s="194"/>
-      <c r="D89" s="195" t="s">
+      <c r="B89" s="159"/>
+      <c r="C89" s="160"/>
+      <c r="D89" s="161" t="s">
         <v>49</v>
       </c>
       <c r="E89" s="117" t="s">
@@ -7515,13 +7515,13 @@
       <c r="W89" s="4"/>
     </row>
     <row r="90" spans="1:36">
-      <c r="A90" s="230"/>
-      <c r="B90" s="193"/>
-      <c r="C90" s="194"/>
-      <c r="D90" s="198" t="s">
+      <c r="A90" s="196"/>
+      <c r="B90" s="159"/>
+      <c r="C90" s="160"/>
+      <c r="D90" s="164" t="s">
         <v>41</v>
       </c>
-      <c r="E90" s="241" t="s">
+      <c r="E90" s="205" t="s">
         <v>231</v>
       </c>
       <c r="F90" s="54" t="s">
@@ -7554,11 +7554,11 @@
       <c r="W90" s="4"/>
     </row>
     <row r="91" spans="1:36" s="24" customFormat="1" ht="16" thickBot="1">
-      <c r="A91" s="242"/>
-      <c r="B91" s="235"/>
-      <c r="C91" s="227"/>
-      <c r="D91" s="235"/>
-      <c r="E91" s="243" t="s">
+      <c r="A91" s="206"/>
+      <c r="B91" s="201"/>
+      <c r="C91" s="193"/>
+      <c r="D91" s="201"/>
+      <c r="E91" s="207" t="s">
         <v>232</v>
       </c>
       <c r="F91" s="73" t="s">
@@ -7592,17 +7592,17 @@
       <c r="Y91" s="25"/>
     </row>
     <row r="92" spans="1:36">
-      <c r="A92" s="237" t="s">
+      <c r="A92" s="203" t="s">
         <v>229</v>
       </c>
-      <c r="B92" s="238" t="s">
+      <c r="B92" s="245" t="s">
         <v>240</v>
       </c>
-      <c r="C92" s="239"/>
-      <c r="D92" s="244" t="s">
+      <c r="C92" s="246"/>
+      <c r="D92" s="208" t="s">
         <v>99</v>
       </c>
-      <c r="E92" s="232" t="s">
+      <c r="E92" s="198" t="s">
         <v>225</v>
       </c>
       <c r="F92" s="32" t="s">
@@ -7635,12 +7635,12 @@
       <c r="W92" s="4"/>
     </row>
     <row r="93" spans="1:36">
-      <c r="A93" s="240" t="s">
+      <c r="A93" s="204" t="s">
         <v>245</v>
       </c>
-      <c r="B93" s="193"/>
-      <c r="C93" s="194"/>
-      <c r="D93" s="195" t="s">
+      <c r="B93" s="159"/>
+      <c r="C93" s="160"/>
+      <c r="D93" s="161" t="s">
         <v>49</v>
       </c>
       <c r="E93" s="117" t="s">
@@ -7670,13 +7670,13 @@
       <c r="W93" s="4"/>
     </row>
     <row r="94" spans="1:36">
-      <c r="A94" s="230"/>
-      <c r="B94" s="193"/>
-      <c r="C94" s="194"/>
-      <c r="D94" s="198" t="s">
+      <c r="A94" s="196"/>
+      <c r="B94" s="159"/>
+      <c r="C94" s="160"/>
+      <c r="D94" s="164" t="s">
         <v>41</v>
       </c>
-      <c r="E94" s="241" t="s">
+      <c r="E94" s="205" t="s">
         <v>231</v>
       </c>
       <c r="F94" s="54" t="s">
@@ -7709,11 +7709,11 @@
       <c r="W94" s="4"/>
     </row>
     <row r="95" spans="1:36" s="24" customFormat="1" ht="16" thickBot="1">
-      <c r="A95" s="242"/>
-      <c r="B95" s="235"/>
-      <c r="C95" s="227"/>
-      <c r="D95" s="235"/>
-      <c r="E95" s="243" t="s">
+      <c r="A95" s="206"/>
+      <c r="B95" s="201"/>
+      <c r="C95" s="193"/>
+      <c r="D95" s="201"/>
+      <c r="E95" s="207" t="s">
         <v>232</v>
       </c>
       <c r="F95" s="73" t="s">
@@ -7747,17 +7747,17 @@
       <c r="Y95" s="25"/>
     </row>
     <row r="96" spans="1:36">
-      <c r="A96" s="237" t="s">
+      <c r="A96" s="203" t="s">
         <v>230</v>
       </c>
-      <c r="B96" s="238" t="s">
+      <c r="B96" s="245" t="s">
         <v>240</v>
       </c>
-      <c r="C96" s="239"/>
-      <c r="D96" s="244" t="s">
+      <c r="C96" s="246"/>
+      <c r="D96" s="208" t="s">
         <v>99</v>
       </c>
-      <c r="E96" s="232" t="s">
+      <c r="E96" s="198" t="s">
         <v>226</v>
       </c>
       <c r="F96" s="32" t="s">
@@ -7790,15 +7790,15 @@
       <c r="W96" s="4"/>
     </row>
     <row r="97" spans="1:25">
-      <c r="A97" s="240" t="s">
+      <c r="A97" s="204" t="s">
         <v>245</v>
       </c>
-      <c r="B97" s="193"/>
-      <c r="C97" s="194"/>
-      <c r="D97" s="195" t="s">
+      <c r="B97" s="159"/>
+      <c r="C97" s="160"/>
+      <c r="D97" s="161" t="s">
         <v>49</v>
       </c>
-      <c r="E97" s="197" t="s">
+      <c r="E97" s="163" t="s">
         <v>236</v>
       </c>
       <c r="F97" s="51" t="s">
@@ -7825,13 +7825,13 @@
       <c r="W97" s="4"/>
     </row>
     <row r="98" spans="1:25">
-      <c r="A98" s="230"/>
-      <c r="B98" s="193"/>
-      <c r="C98" s="194"/>
-      <c r="D98" s="198" t="s">
+      <c r="A98" s="196"/>
+      <c r="B98" s="159"/>
+      <c r="C98" s="160"/>
+      <c r="D98" s="164" t="s">
         <v>41</v>
       </c>
-      <c r="E98" s="241" t="s">
+      <c r="E98" s="205" t="s">
         <v>231</v>
       </c>
       <c r="F98" s="54" t="s">
@@ -7864,11 +7864,11 @@
       <c r="W98" s="4"/>
     </row>
     <row r="99" spans="1:25" s="24" customFormat="1" ht="16" thickBot="1">
-      <c r="A99" s="242"/>
-      <c r="B99" s="235"/>
-      <c r="C99" s="227"/>
-      <c r="D99" s="245"/>
-      <c r="E99" s="243" t="s">
+      <c r="A99" s="206"/>
+      <c r="B99" s="201"/>
+      <c r="C99" s="193"/>
+      <c r="D99" s="209"/>
+      <c r="E99" s="207" t="s">
         <v>232</v>
       </c>
       <c r="F99" s="55" t="s">
@@ -7902,19 +7902,19 @@
       <c r="Y99" s="25"/>
     </row>
     <row r="100" spans="1:25" s="8" customFormat="1">
-      <c r="A100" s="192" t="s">
+      <c r="A100" s="158" t="s">
         <v>19</v>
       </c>
-      <c r="B100" s="193" t="s">
+      <c r="B100" s="159" t="s">
         <v>148</v>
       </c>
-      <c r="C100" s="194">
+      <c r="C100" s="160">
         <v>19</v>
       </c>
-      <c r="D100" s="195" t="s">
+      <c r="D100" s="161" t="s">
         <v>100</v>
       </c>
-      <c r="E100" s="197" t="s">
+      <c r="E100" s="163" t="s">
         <v>106</v>
       </c>
       <c r="F100" s="31" t="s">
@@ -7966,19 +7966,19 @@
       <c r="Y100" s="9"/>
     </row>
     <row r="101" spans="1:25" s="16" customFormat="1" ht="16" thickBot="1">
-      <c r="A101" s="246" t="s">
+      <c r="A101" s="210" t="s">
         <v>20</v>
       </c>
-      <c r="B101" s="235" t="s">
+      <c r="B101" s="201" t="s">
         <v>148</v>
       </c>
-      <c r="C101" s="227">
+      <c r="C101" s="193">
         <v>20</v>
       </c>
-      <c r="D101" s="235" t="s">
+      <c r="D101" s="201" t="s">
         <v>100</v>
       </c>
-      <c r="E101" s="236" t="s">
+      <c r="E101" s="202" t="s">
         <v>107</v>
       </c>
       <c r="F101" s="50" t="s">
@@ -8030,17 +8030,17 @@
       <c r="Y101" s="15"/>
     </row>
     <row r="102" spans="1:25" s="3" customFormat="1">
-      <c r="A102" s="192" t="s">
+      <c r="A102" s="158" t="s">
         <v>292</v>
       </c>
-      <c r="B102" s="193"/>
-      <c r="C102" s="194" t="s">
+      <c r="B102" s="159"/>
+      <c r="C102" s="160" t="s">
         <v>293</v>
       </c>
-      <c r="D102" s="193" t="s">
+      <c r="D102" s="159" t="s">
         <v>306</v>
       </c>
-      <c r="E102" s="197"/>
+      <c r="E102" s="163"/>
       <c r="F102" s="10"/>
       <c r="G102" s="4"/>
       <c r="H102" s="10"/>
@@ -8066,19 +8066,19 @@
       <c r="Y102" s="9"/>
     </row>
     <row r="103" spans="1:25" s="8" customFormat="1">
-      <c r="A103" s="192" t="s">
+      <c r="A103" s="158" t="s">
         <v>21</v>
       </c>
-      <c r="B103" s="193" t="s">
+      <c r="B103" s="159" t="s">
         <v>149</v>
       </c>
-      <c r="C103" s="194">
+      <c r="C103" s="160">
         <v>23</v>
       </c>
-      <c r="D103" s="195" t="s">
+      <c r="D103" s="161" t="s">
         <v>563</v>
       </c>
-      <c r="E103" s="197" t="s">
+      <c r="E103" s="163" t="s">
         <v>128</v>
       </c>
       <c r="F103" s="31" t="s">
@@ -8122,19 +8122,19 @@
       <c r="Y103" s="9"/>
     </row>
     <row r="104" spans="1:25" s="8" customFormat="1">
-      <c r="A104" s="192" t="s">
+      <c r="A104" s="158" t="s">
         <v>22</v>
       </c>
-      <c r="B104" s="193" t="s">
+      <c r="B104" s="159" t="s">
         <v>149</v>
       </c>
-      <c r="C104" s="194">
+      <c r="C104" s="160">
         <v>24</v>
       </c>
-      <c r="D104" s="195" t="s">
+      <c r="D104" s="161" t="s">
         <v>564</v>
       </c>
-      <c r="E104" s="197" t="s">
+      <c r="E104" s="163" t="s">
         <v>130</v>
       </c>
       <c r="F104" s="31" t="s">
@@ -8176,19 +8176,19 @@
       <c r="Y104" s="9"/>
     </row>
     <row r="105" spans="1:25" s="8" customFormat="1">
-      <c r="A105" s="192" t="s">
+      <c r="A105" s="158" t="s">
         <v>23</v>
       </c>
-      <c r="B105" s="193" t="s">
+      <c r="B105" s="159" t="s">
         <v>149</v>
       </c>
-      <c r="C105" s="194">
+      <c r="C105" s="160">
         <v>25</v>
       </c>
-      <c r="D105" s="195" t="s">
+      <c r="D105" s="161" t="s">
         <v>565</v>
       </c>
-      <c r="E105" s="197" t="s">
+      <c r="E105" s="163" t="s">
         <v>137</v>
       </c>
       <c r="F105" s="31" t="s">
@@ -8248,7 +8248,7 @@
       <c r="B106" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="C106" s="191">
+      <c r="C106" s="157">
         <v>28</v>
       </c>
       <c r="D106" s="5"/>
@@ -8338,12 +8338,12 @@
       </c>
       <c r="I108" s="4"/>
       <c r="J108" s="109"/>
-      <c r="K108" s="172" t="s">
+      <c r="K108" s="233" t="s">
         <v>457</v>
       </c>
-      <c r="L108" s="173"/>
-      <c r="M108" s="174"/>
-      <c r="N108" s="169" t="s">
+      <c r="L108" s="234"/>
+      <c r="M108" s="235"/>
+      <c r="N108" s="230" t="s">
         <v>464</v>
       </c>
       <c r="O108" s="4"/>
@@ -8371,10 +8371,10 @@
       <c r="H109" s="5"/>
       <c r="I109" s="4"/>
       <c r="J109" s="109"/>
-      <c r="K109" s="175"/>
-      <c r="L109" s="176"/>
-      <c r="M109" s="177"/>
-      <c r="N109" s="170"/>
+      <c r="K109" s="236"/>
+      <c r="L109" s="237"/>
+      <c r="M109" s="238"/>
+      <c r="N109" s="231"/>
       <c r="O109" s="4"/>
       <c r="P109" s="5"/>
       <c r="Q109" s="4"/>
@@ -8402,10 +8402,10 @@
       </c>
       <c r="I110" s="4"/>
       <c r="J110" s="109"/>
-      <c r="K110" s="175"/>
-      <c r="L110" s="176"/>
-      <c r="M110" s="177"/>
-      <c r="N110" s="170"/>
+      <c r="K110" s="236"/>
+      <c r="L110" s="237"/>
+      <c r="M110" s="238"/>
+      <c r="N110" s="231"/>
       <c r="O110" s="4"/>
       <c r="P110" s="5"/>
       <c r="Q110" s="4"/>
@@ -8433,10 +8433,10 @@
       <c r="J111" s="110" t="s">
         <v>361</v>
       </c>
-      <c r="K111" s="178"/>
-      <c r="L111" s="179"/>
-      <c r="M111" s="180"/>
-      <c r="N111" s="171"/>
+      <c r="K111" s="239"/>
+      <c r="L111" s="240"/>
+      <c r="M111" s="241"/>
+      <c r="N111" s="232"/>
       <c r="O111" s="18"/>
       <c r="P111" s="17"/>
       <c r="Q111" s="18"/>
@@ -8455,7 +8455,7 @@
       <c r="B112" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="C112" s="191">
+      <c r="C112" s="157">
         <v>36</v>
       </c>
       <c r="D112" s="5"/>
@@ -8495,19 +8495,19 @@
       <c r="Y112" s="9"/>
     </row>
     <row r="113" spans="1:25">
-      <c r="A113" s="192" t="s">
+      <c r="A113" s="158" t="s">
         <v>25</v>
       </c>
-      <c r="B113" s="193" t="s">
+      <c r="B113" s="159" t="s">
         <v>148</v>
       </c>
-      <c r="C113" s="194">
+      <c r="C113" s="160">
         <v>37</v>
       </c>
-      <c r="D113" s="195" t="s">
+      <c r="D113" s="161" t="s">
         <v>100</v>
       </c>
-      <c r="E113" s="197" t="s">
+      <c r="E113" s="163" t="s">
         <v>182</v>
       </c>
       <c r="F113" s="31" t="s">
@@ -8546,19 +8546,19 @@
       <c r="W113" s="4"/>
     </row>
     <row r="114" spans="1:25" s="24" customFormat="1" ht="16" thickBot="1">
-      <c r="A114" s="246" t="s">
+      <c r="A114" s="210" t="s">
         <v>26</v>
       </c>
-      <c r="B114" s="235" t="s">
+      <c r="B114" s="201" t="s">
         <v>148</v>
       </c>
-      <c r="C114" s="227">
+      <c r="C114" s="193">
         <v>38</v>
       </c>
-      <c r="D114" s="235" t="s">
+      <c r="D114" s="201" t="s">
         <v>100</v>
       </c>
-      <c r="E114" s="236" t="s">
+      <c r="E114" s="202" t="s">
         <v>144</v>
       </c>
       <c r="F114" s="50" t="s">
@@ -8608,19 +8608,19 @@
       <c r="Y114" s="25"/>
     </row>
     <row r="115" spans="1:25">
-      <c r="A115" s="192" t="s">
+      <c r="A115" s="158" t="s">
         <v>27</v>
       </c>
-      <c r="B115" s="193" t="s">
+      <c r="B115" s="159" t="s">
         <v>161</v>
       </c>
-      <c r="C115" s="194">
+      <c r="C115" s="160">
         <v>39</v>
       </c>
-      <c r="D115" s="254" t="s">
+      <c r="D115" s="218" t="s">
         <v>544</v>
       </c>
-      <c r="E115" s="197" t="s">
+      <c r="E115" s="163" t="s">
         <v>209</v>
       </c>
       <c r="F115" s="31" t="s">
@@ -8659,13 +8659,13 @@
       <c r="W115" s="4"/>
     </row>
     <row r="116" spans="1:25">
-      <c r="A116" s="192"/>
-      <c r="B116" s="193"/>
-      <c r="C116" s="194"/>
-      <c r="D116" s="254" t="s">
+      <c r="A116" s="158"/>
+      <c r="B116" s="159"/>
+      <c r="C116" s="160"/>
+      <c r="D116" s="218" t="s">
         <v>550</v>
       </c>
-      <c r="E116" s="197" t="s">
+      <c r="E116" s="163" t="s">
         <v>217</v>
       </c>
       <c r="F116" s="31"/>
@@ -8688,13 +8688,13 @@
       <c r="W116" s="4"/>
     </row>
     <row r="117" spans="1:25">
-      <c r="A117" s="192"/>
-      <c r="B117" s="193"/>
-      <c r="C117" s="194"/>
-      <c r="D117" s="254" t="s">
+      <c r="A117" s="158"/>
+      <c r="B117" s="159"/>
+      <c r="C117" s="160"/>
+      <c r="D117" s="218" t="s">
         <v>551</v>
       </c>
-      <c r="E117" s="197" t="s">
+      <c r="E117" s="163" t="s">
         <v>218</v>
       </c>
       <c r="F117" s="31"/>
@@ -8717,13 +8717,13 @@
       <c r="W117" s="4"/>
     </row>
     <row r="118" spans="1:25">
-      <c r="A118" s="197"/>
-      <c r="B118" s="193"/>
-      <c r="C118" s="194"/>
-      <c r="D118" s="254" t="s">
+      <c r="A118" s="163"/>
+      <c r="B118" s="159"/>
+      <c r="C118" s="160"/>
+      <c r="D118" s="218" t="s">
         <v>545</v>
       </c>
-      <c r="E118" s="197" t="s">
+      <c r="E118" s="163" t="s">
         <v>184</v>
       </c>
       <c r="F118" s="31" t="s">
@@ -8764,13 +8764,13 @@
       <c r="W118" s="4"/>
     </row>
     <row r="119" spans="1:25">
-      <c r="A119" s="197"/>
-      <c r="B119" s="193"/>
-      <c r="C119" s="194"/>
-      <c r="D119" s="254" t="s">
+      <c r="A119" s="163"/>
+      <c r="B119" s="159"/>
+      <c r="C119" s="160"/>
+      <c r="D119" s="218" t="s">
         <v>552</v>
       </c>
-      <c r="E119" s="197"/>
+      <c r="E119" s="163"/>
       <c r="F119" s="31"/>
       <c r="G119" s="4"/>
       <c r="H119" s="5"/>
@@ -8791,13 +8791,13 @@
       <c r="W119" s="4"/>
     </row>
     <row r="120" spans="1:25">
-      <c r="A120" s="197"/>
-      <c r="B120" s="193"/>
-      <c r="C120" s="194"/>
-      <c r="D120" s="254" t="s">
+      <c r="A120" s="163"/>
+      <c r="B120" s="159"/>
+      <c r="C120" s="160"/>
+      <c r="D120" s="218" t="s">
         <v>546</v>
       </c>
-      <c r="E120" s="197" t="s">
+      <c r="E120" s="163" t="s">
         <v>184</v>
       </c>
       <c r="F120" s="31" t="s">
@@ -8836,13 +8836,13 @@
       <c r="W120" s="4"/>
     </row>
     <row r="121" spans="1:25">
-      <c r="A121" s="197"/>
-      <c r="B121" s="193"/>
-      <c r="C121" s="194"/>
-      <c r="D121" s="254" t="s">
+      <c r="A121" s="163"/>
+      <c r="B121" s="159"/>
+      <c r="C121" s="160"/>
+      <c r="D121" s="218" t="s">
         <v>552</v>
       </c>
-      <c r="E121" s="197"/>
+      <c r="E121" s="163"/>
       <c r="F121" s="31"/>
       <c r="G121" s="4"/>
       <c r="H121" s="5"/>
@@ -8863,13 +8863,13 @@
       <c r="W121" s="4"/>
     </row>
     <row r="122" spans="1:25">
-      <c r="A122" s="197"/>
-      <c r="B122" s="193"/>
-      <c r="C122" s="194"/>
-      <c r="D122" s="254" t="s">
+      <c r="A122" s="163"/>
+      <c r="B122" s="159"/>
+      <c r="C122" s="160"/>
+      <c r="D122" s="218" t="s">
         <v>547</v>
       </c>
-      <c r="E122" s="197" t="s">
+      <c r="E122" s="163" t="s">
         <v>184</v>
       </c>
       <c r="F122" s="31" t="s">
@@ -8907,18 +8907,18 @@
       <c r="V122" s="49" t="s">
         <v>444</v>
       </c>
-      <c r="W122" s="183" t="s">
+      <c r="W122" s="244" t="s">
         <v>507</v>
       </c>
     </row>
     <row r="123" spans="1:25">
-      <c r="A123" s="197"/>
-      <c r="B123" s="193"/>
-      <c r="C123" s="194"/>
-      <c r="D123" s="254" t="s">
+      <c r="A123" s="163"/>
+      <c r="B123" s="159"/>
+      <c r="C123" s="160"/>
+      <c r="D123" s="218" t="s">
         <v>552</v>
       </c>
-      <c r="E123" s="197"/>
+      <c r="E123" s="163"/>
       <c r="F123" s="31"/>
       <c r="G123" s="33"/>
       <c r="H123" s="31"/>
@@ -8936,16 +8936,16 @@
       <c r="T123" s="31"/>
       <c r="U123" s="33"/>
       <c r="V123" s="49"/>
-      <c r="W123" s="183"/>
+      <c r="W123" s="244"/>
     </row>
     <row r="124" spans="1:25">
-      <c r="A124" s="197"/>
-      <c r="B124" s="193"/>
-      <c r="C124" s="194"/>
-      <c r="D124" s="254" t="s">
+      <c r="A124" s="163"/>
+      <c r="B124" s="159"/>
+      <c r="C124" s="160"/>
+      <c r="D124" s="218" t="s">
         <v>548</v>
       </c>
-      <c r="E124" s="197" t="s">
+      <c r="E124" s="163" t="s">
         <v>184</v>
       </c>
       <c r="F124" s="10"/>
@@ -8971,16 +8971,16 @@
       <c r="V124" s="49" t="s">
         <v>445</v>
       </c>
-      <c r="W124" s="183"/>
+      <c r="W124" s="244"/>
     </row>
     <row r="125" spans="1:25">
-      <c r="A125" s="197"/>
-      <c r="B125" s="193"/>
-      <c r="C125" s="194"/>
-      <c r="D125" s="254" t="s">
+      <c r="A125" s="163"/>
+      <c r="B125" s="159"/>
+      <c r="C125" s="160"/>
+      <c r="D125" s="218" t="s">
         <v>552</v>
       </c>
-      <c r="E125" s="197"/>
+      <c r="E125" s="163"/>
       <c r="F125" s="10"/>
       <c r="G125" s="57"/>
       <c r="H125" s="5"/>
@@ -8998,16 +8998,16 @@
       <c r="T125" s="31"/>
       <c r="U125" s="33"/>
       <c r="V125" s="49"/>
-      <c r="W125" s="183"/>
+      <c r="W125" s="244"/>
     </row>
     <row r="126" spans="1:25">
-      <c r="A126" s="197"/>
-      <c r="B126" s="193"/>
-      <c r="C126" s="194"/>
-      <c r="D126" s="254" t="s">
+      <c r="A126" s="163"/>
+      <c r="B126" s="159"/>
+      <c r="C126" s="160"/>
+      <c r="D126" s="218" t="s">
         <v>549</v>
       </c>
-      <c r="E126" s="197" t="s">
+      <c r="E126" s="163" t="s">
         <v>184</v>
       </c>
       <c r="F126" s="10"/>
@@ -9033,16 +9033,16 @@
       <c r="V126" s="49" t="s">
         <v>446</v>
       </c>
-      <c r="W126" s="183"/>
+      <c r="W126" s="244"/>
     </row>
     <row r="127" spans="1:25">
-      <c r="A127" s="197"/>
-      <c r="B127" s="193"/>
-      <c r="C127" s="194"/>
-      <c r="D127" s="254" t="s">
+      <c r="A127" s="163"/>
+      <c r="B127" s="159"/>
+      <c r="C127" s="160"/>
+      <c r="D127" s="218" t="s">
         <v>552</v>
       </c>
-      <c r="E127" s="197"/>
+      <c r="E127" s="163"/>
       <c r="F127" s="10"/>
       <c r="G127" s="4"/>
       <c r="H127" s="5"/>
@@ -9060,16 +9060,16 @@
       <c r="T127" s="31"/>
       <c r="U127" s="33"/>
       <c r="V127" s="49"/>
-      <c r="W127" s="183"/>
+      <c r="W127" s="244"/>
     </row>
     <row r="128" spans="1:25">
-      <c r="A128" s="197"/>
-      <c r="B128" s="193"/>
-      <c r="C128" s="194"/>
-      <c r="D128" s="250" t="s">
+      <c r="A128" s="163"/>
+      <c r="B128" s="159"/>
+      <c r="C128" s="160"/>
+      <c r="D128" s="214" t="s">
         <v>100</v>
       </c>
-      <c r="E128" s="251" t="s">
+      <c r="E128" s="215" t="s">
         <v>184</v>
       </c>
       <c r="F128" s="10"/>
@@ -9095,16 +9095,16 @@
       <c r="V128" s="49" t="s">
         <v>448</v>
       </c>
-      <c r="W128" s="183"/>
+      <c r="W128" s="244"/>
     </row>
     <row r="129" spans="1:25" s="24" customFormat="1" ht="16" thickBot="1">
-      <c r="A129" s="236"/>
-      <c r="B129" s="235"/>
-      <c r="C129" s="227"/>
-      <c r="D129" s="252" t="s">
+      <c r="A129" s="202"/>
+      <c r="B129" s="201"/>
+      <c r="C129" s="193"/>
+      <c r="D129" s="216" t="s">
         <v>100</v>
       </c>
-      <c r="E129" s="253" t="s">
+      <c r="E129" s="217" t="s">
         <v>184</v>
       </c>
       <c r="F129" s="17"/>
@@ -9128,19 +9128,19 @@
       <c r="Y129" s="25"/>
     </row>
     <row r="130" spans="1:25">
-      <c r="A130" s="192" t="s">
+      <c r="A130" s="158" t="s">
         <v>28</v>
       </c>
-      <c r="B130" s="193" t="s">
+      <c r="B130" s="159" t="s">
         <v>161</v>
       </c>
-      <c r="C130" s="194">
+      <c r="C130" s="160">
         <v>40</v>
       </c>
-      <c r="D130" s="254" t="s">
+      <c r="D130" s="218" t="s">
         <v>557</v>
       </c>
-      <c r="E130" s="197" t="s">
+      <c r="E130" s="163" t="s">
         <v>432</v>
       </c>
       <c r="F130" s="31" t="s">
@@ -9159,7 +9159,7 @@
       <c r="M130" s="48" t="s">
         <v>449</v>
       </c>
-      <c r="N130" s="169" t="s">
+      <c r="N130" s="230" t="s">
         <v>466</v>
       </c>
       <c r="O130" s="4"/>
@@ -9173,13 +9173,13 @@
       <c r="W130" s="4"/>
     </row>
     <row r="131" spans="1:25">
-      <c r="A131" s="192"/>
-      <c r="B131" s="193"/>
-      <c r="C131" s="194"/>
-      <c r="D131" s="254" t="s">
+      <c r="A131" s="158"/>
+      <c r="B131" s="159"/>
+      <c r="C131" s="160"/>
+      <c r="D131" s="218" t="s">
         <v>558</v>
       </c>
-      <c r="E131" s="197" t="s">
+      <c r="E131" s="163" t="s">
         <v>553</v>
       </c>
       <c r="F131" s="31"/>
@@ -9190,7 +9190,7 @@
       <c r="K131" s="49"/>
       <c r="L131" s="48"/>
       <c r="M131" s="48"/>
-      <c r="N131" s="170"/>
+      <c r="N131" s="231"/>
       <c r="O131" s="4"/>
       <c r="P131" s="5"/>
       <c r="Q131" s="4"/>
@@ -9202,13 +9202,13 @@
       <c r="W131" s="4"/>
     </row>
     <row r="132" spans="1:25">
-      <c r="A132" s="192"/>
-      <c r="B132" s="193"/>
-      <c r="C132" s="194"/>
-      <c r="D132" s="254" t="s">
+      <c r="A132" s="158"/>
+      <c r="B132" s="159"/>
+      <c r="C132" s="160"/>
+      <c r="D132" s="218" t="s">
         <v>559</v>
       </c>
-      <c r="E132" s="197" t="s">
+      <c r="E132" s="163" t="s">
         <v>554</v>
       </c>
       <c r="F132" s="31"/>
@@ -9219,7 +9219,7 @@
       <c r="K132" s="49"/>
       <c r="L132" s="48"/>
       <c r="M132" s="48"/>
-      <c r="N132" s="170"/>
+      <c r="N132" s="231"/>
       <c r="O132" s="4"/>
       <c r="P132" s="5"/>
       <c r="Q132" s="4"/>
@@ -9231,13 +9231,13 @@
       <c r="W132" s="4"/>
     </row>
     <row r="133" spans="1:25">
-      <c r="A133" s="197"/>
-      <c r="B133" s="193"/>
-      <c r="C133" s="194"/>
-      <c r="D133" s="195" t="s">
+      <c r="A133" s="163"/>
+      <c r="B133" s="159"/>
+      <c r="C133" s="160"/>
+      <c r="D133" s="161" t="s">
         <v>100</v>
       </c>
-      <c r="E133" s="197" t="s">
+      <c r="E133" s="163" t="s">
         <v>185</v>
       </c>
       <c r="F133" s="32" t="s">
@@ -9256,7 +9256,7 @@
       <c r="M133" s="48" t="s">
         <v>450</v>
       </c>
-      <c r="N133" s="170"/>
+      <c r="N133" s="231"/>
       <c r="O133" s="4"/>
       <c r="P133" s="5"/>
       <c r="Q133" s="4"/>
@@ -9268,13 +9268,13 @@
       <c r="W133" s="4"/>
     </row>
     <row r="134" spans="1:25">
-      <c r="A134" s="197"/>
-      <c r="B134" s="193"/>
-      <c r="C134" s="194"/>
-      <c r="D134" s="254" t="s">
+      <c r="A134" s="163"/>
+      <c r="B134" s="159"/>
+      <c r="C134" s="160"/>
+      <c r="D134" s="218" t="s">
         <v>552</v>
       </c>
-      <c r="E134" s="197"/>
+      <c r="E134" s="163"/>
       <c r="F134" s="32"/>
       <c r="G134" s="4"/>
       <c r="H134" s="5"/>
@@ -9283,7 +9283,7 @@
       <c r="K134" s="49"/>
       <c r="L134" s="48"/>
       <c r="M134" s="48"/>
-      <c r="N134" s="170"/>
+      <c r="N134" s="231"/>
       <c r="O134" s="4"/>
       <c r="P134" s="5"/>
       <c r="Q134" s="4"/>
@@ -9295,13 +9295,13 @@
       <c r="W134" s="4"/>
     </row>
     <row r="135" spans="1:25">
-      <c r="A135" s="197"/>
-      <c r="B135" s="193"/>
-      <c r="C135" s="194"/>
-      <c r="D135" s="195" t="s">
+      <c r="A135" s="163"/>
+      <c r="B135" s="159"/>
+      <c r="C135" s="160"/>
+      <c r="D135" s="161" t="s">
         <v>100</v>
       </c>
-      <c r="E135" s="197" t="s">
+      <c r="E135" s="163" t="s">
         <v>185</v>
       </c>
       <c r="F135" s="32" t="s">
@@ -9320,7 +9320,7 @@
       <c r="M135" s="48" t="s">
         <v>451</v>
       </c>
-      <c r="N135" s="170"/>
+      <c r="N135" s="231"/>
       <c r="O135" s="4"/>
       <c r="P135" s="5"/>
       <c r="Q135" s="4"/>
@@ -9332,13 +9332,13 @@
       <c r="W135" s="4"/>
     </row>
     <row r="136" spans="1:25">
-      <c r="A136" s="197"/>
-      <c r="B136" s="193"/>
-      <c r="C136" s="194"/>
-      <c r="D136" s="254" t="s">
+      <c r="A136" s="163"/>
+      <c r="B136" s="159"/>
+      <c r="C136" s="160"/>
+      <c r="D136" s="218" t="s">
         <v>552</v>
       </c>
-      <c r="E136" s="197"/>
+      <c r="E136" s="163"/>
       <c r="F136" s="32"/>
       <c r="G136" s="4"/>
       <c r="H136" s="5"/>
@@ -9347,7 +9347,7 @@
       <c r="K136" s="49"/>
       <c r="L136" s="48"/>
       <c r="M136" s="48"/>
-      <c r="N136" s="170"/>
+      <c r="N136" s="231"/>
       <c r="O136" s="4"/>
       <c r="P136" s="5"/>
       <c r="Q136" s="4"/>
@@ -9359,13 +9359,13 @@
       <c r="W136" s="4"/>
     </row>
     <row r="137" spans="1:25">
-      <c r="A137" s="197"/>
-      <c r="B137" s="193"/>
-      <c r="C137" s="194"/>
-      <c r="D137" s="195" t="s">
+      <c r="A137" s="163"/>
+      <c r="B137" s="159"/>
+      <c r="C137" s="160"/>
+      <c r="D137" s="161" t="s">
         <v>100</v>
       </c>
-      <c r="E137" s="197" t="s">
+      <c r="E137" s="163" t="s">
         <v>185</v>
       </c>
       <c r="F137" s="31" t="s">
@@ -9388,7 +9388,7 @@
       <c r="M137" s="48" t="s">
         <v>452</v>
       </c>
-      <c r="N137" s="170"/>
+      <c r="N137" s="231"/>
       <c r="O137" s="4"/>
       <c r="P137" s="5"/>
       <c r="Q137" s="4"/>
@@ -9400,13 +9400,13 @@
       <c r="W137" s="4"/>
     </row>
     <row r="138" spans="1:25">
-      <c r="A138" s="197"/>
-      <c r="B138" s="193"/>
-      <c r="C138" s="194"/>
-      <c r="D138" s="254" t="s">
+      <c r="A138" s="163"/>
+      <c r="B138" s="159"/>
+      <c r="C138" s="160"/>
+      <c r="D138" s="218" t="s">
         <v>552</v>
       </c>
-      <c r="E138" s="197"/>
+      <c r="E138" s="163"/>
       <c r="F138" s="31"/>
       <c r="G138" s="33"/>
       <c r="H138" s="31"/>
@@ -9415,7 +9415,7 @@
       <c r="K138" s="49"/>
       <c r="L138" s="48"/>
       <c r="M138" s="48"/>
-      <c r="N138" s="170"/>
+      <c r="N138" s="231"/>
       <c r="O138" s="4"/>
       <c r="P138" s="5"/>
       <c r="Q138" s="4"/>
@@ -9427,13 +9427,13 @@
       <c r="W138" s="4"/>
     </row>
     <row r="139" spans="1:25">
-      <c r="A139" s="197"/>
-      <c r="B139" s="193"/>
-      <c r="C139" s="194"/>
-      <c r="D139" s="195" t="s">
+      <c r="A139" s="163"/>
+      <c r="B139" s="159"/>
+      <c r="C139" s="160"/>
+      <c r="D139" s="161" t="s">
         <v>100</v>
       </c>
-      <c r="E139" s="197" t="s">
+      <c r="E139" s="163" t="s">
         <v>185</v>
       </c>
       <c r="F139" s="31"/>
@@ -9444,7 +9444,7 @@
       <c r="K139" s="49"/>
       <c r="L139" s="48"/>
       <c r="M139" s="48"/>
-      <c r="N139" s="170"/>
+      <c r="N139" s="231"/>
       <c r="O139" s="4"/>
       <c r="P139" s="5"/>
       <c r="Q139" s="4"/>
@@ -9456,13 +9456,13 @@
       <c r="W139" s="4"/>
     </row>
     <row r="140" spans="1:25" s="24" customFormat="1" ht="16" thickBot="1">
-      <c r="A140" s="236"/>
-      <c r="B140" s="235"/>
-      <c r="C140" s="227"/>
-      <c r="D140" s="255" t="s">
+      <c r="A140" s="202"/>
+      <c r="B140" s="201"/>
+      <c r="C140" s="193"/>
+      <c r="D140" s="219" t="s">
         <v>552</v>
       </c>
-      <c r="E140" s="236"/>
+      <c r="E140" s="202"/>
       <c r="F140" s="17"/>
       <c r="G140" s="18"/>
       <c r="H140" s="17"/>
@@ -9471,7 +9471,7 @@
       <c r="K140" s="120"/>
       <c r="L140" s="89"/>
       <c r="M140" s="89"/>
-      <c r="N140" s="171"/>
+      <c r="N140" s="232"/>
       <c r="O140" s="18"/>
       <c r="P140" s="17"/>
       <c r="Q140" s="18"/>
@@ -9484,19 +9484,19 @@
       <c r="Y140" s="25"/>
     </row>
     <row r="141" spans="1:25">
-      <c r="A141" s="192" t="s">
+      <c r="A141" s="158" t="s">
         <v>29</v>
       </c>
-      <c r="B141" s="193" t="s">
+      <c r="B141" s="159" t="s">
         <v>161</v>
       </c>
-      <c r="C141" s="194">
+      <c r="C141" s="160">
         <v>41</v>
       </c>
-      <c r="D141" s="254" t="s">
+      <c r="D141" s="218" t="s">
         <v>560</v>
       </c>
-      <c r="E141" s="197" t="s">
+      <c r="E141" s="163" t="s">
         <v>441</v>
       </c>
       <c r="F141" s="31" t="s">
@@ -9515,7 +9515,7 @@
       <c r="M141" s="48" t="s">
         <v>453</v>
       </c>
-      <c r="N141" s="169" t="s">
+      <c r="N141" s="230" t="s">
         <v>467</v>
       </c>
       <c r="O141" s="4"/>
@@ -9529,13 +9529,13 @@
       <c r="W141" s="4"/>
     </row>
     <row r="142" spans="1:25">
-      <c r="A142" s="192"/>
-      <c r="B142" s="193"/>
-      <c r="C142" s="194"/>
-      <c r="D142" s="254" t="s">
+      <c r="A142" s="158"/>
+      <c r="B142" s="159"/>
+      <c r="C142" s="160"/>
+      <c r="D142" s="218" t="s">
         <v>561</v>
       </c>
-      <c r="E142" s="197" t="s">
+      <c r="E142" s="163" t="s">
         <v>555</v>
       </c>
       <c r="F142" s="31"/>
@@ -9546,7 +9546,7 @@
       <c r="K142" s="49"/>
       <c r="L142" s="48"/>
       <c r="M142" s="48"/>
-      <c r="N142" s="170"/>
+      <c r="N142" s="231"/>
       <c r="O142" s="4"/>
       <c r="P142" s="5"/>
       <c r="Q142" s="4"/>
@@ -9558,13 +9558,13 @@
       <c r="W142" s="4"/>
     </row>
     <row r="143" spans="1:25">
-      <c r="A143" s="192"/>
-      <c r="B143" s="193"/>
-      <c r="C143" s="194"/>
-      <c r="D143" s="254" t="s">
+      <c r="A143" s="158"/>
+      <c r="B143" s="159"/>
+      <c r="C143" s="160"/>
+      <c r="D143" s="218" t="s">
         <v>562</v>
       </c>
-      <c r="E143" s="197" t="s">
+      <c r="E143" s="163" t="s">
         <v>556</v>
       </c>
       <c r="F143" s="31"/>
@@ -9575,7 +9575,7 @@
       <c r="K143" s="49"/>
       <c r="L143" s="48"/>
       <c r="M143" s="48"/>
-      <c r="N143" s="170"/>
+      <c r="N143" s="231"/>
       <c r="O143" s="4"/>
       <c r="P143" s="5"/>
       <c r="Q143" s="4"/>
@@ -9587,13 +9587,13 @@
       <c r="W143" s="4"/>
     </row>
     <row r="144" spans="1:25">
-      <c r="A144" s="197"/>
-      <c r="B144" s="193"/>
-      <c r="C144" s="194"/>
-      <c r="D144" s="195" t="s">
+      <c r="A144" s="163"/>
+      <c r="B144" s="159"/>
+      <c r="C144" s="160"/>
+      <c r="D144" s="161" t="s">
         <v>100</v>
       </c>
-      <c r="E144" s="197" t="s">
+      <c r="E144" s="163" t="s">
         <v>186</v>
       </c>
       <c r="F144" s="31" t="s">
@@ -9612,7 +9612,7 @@
       <c r="M144" s="48" t="s">
         <v>454</v>
       </c>
-      <c r="N144" s="170"/>
+      <c r="N144" s="231"/>
       <c r="O144" s="4"/>
       <c r="P144" s="5"/>
       <c r="Q144" s="4"/>
@@ -9624,13 +9624,13 @@
       <c r="W144" s="4"/>
     </row>
     <row r="145" spans="1:25">
-      <c r="A145" s="197"/>
-      <c r="B145" s="193"/>
-      <c r="C145" s="194"/>
-      <c r="D145" s="254" t="s">
+      <c r="A145" s="163"/>
+      <c r="B145" s="159"/>
+      <c r="C145" s="160"/>
+      <c r="D145" s="218" t="s">
         <v>552</v>
       </c>
-      <c r="E145" s="197"/>
+      <c r="E145" s="163"/>
       <c r="F145" s="31"/>
       <c r="G145" s="4"/>
       <c r="H145" s="5"/>
@@ -9639,7 +9639,7 @@
       <c r="K145" s="49"/>
       <c r="L145" s="48"/>
       <c r="M145" s="48"/>
-      <c r="N145" s="170"/>
+      <c r="N145" s="231"/>
       <c r="O145" s="4"/>
       <c r="P145" s="5"/>
       <c r="Q145" s="4"/>
@@ -9651,13 +9651,13 @@
       <c r="W145" s="4"/>
     </row>
     <row r="146" spans="1:25">
-      <c r="A146" s="197"/>
-      <c r="B146" s="193"/>
-      <c r="C146" s="194"/>
-      <c r="D146" s="195" t="s">
+      <c r="A146" s="163"/>
+      <c r="B146" s="159"/>
+      <c r="C146" s="160"/>
+      <c r="D146" s="161" t="s">
         <v>100</v>
       </c>
-      <c r="E146" s="197" t="s">
+      <c r="E146" s="163" t="s">
         <v>186</v>
       </c>
       <c r="F146" s="31" t="s">
@@ -9676,7 +9676,7 @@
       <c r="M146" s="48" t="s">
         <v>455</v>
       </c>
-      <c r="N146" s="170"/>
+      <c r="N146" s="231"/>
       <c r="O146" s="4"/>
       <c r="P146" s="5"/>
       <c r="Q146" s="4"/>
@@ -9688,13 +9688,13 @@
       <c r="W146" s="4"/>
     </row>
     <row r="147" spans="1:25">
-      <c r="A147" s="197"/>
-      <c r="B147" s="193"/>
-      <c r="C147" s="194"/>
-      <c r="D147" s="254" t="s">
+      <c r="A147" s="163"/>
+      <c r="B147" s="159"/>
+      <c r="C147" s="160"/>
+      <c r="D147" s="218" t="s">
         <v>552</v>
       </c>
-      <c r="E147" s="197"/>
+      <c r="E147" s="163"/>
       <c r="F147" s="31"/>
       <c r="G147" s="4"/>
       <c r="H147" s="5"/>
@@ -9703,7 +9703,7 @@
       <c r="K147" s="49"/>
       <c r="L147" s="48"/>
       <c r="M147" s="48"/>
-      <c r="N147" s="170"/>
+      <c r="N147" s="231"/>
       <c r="O147" s="4"/>
       <c r="P147" s="5"/>
       <c r="Q147" s="4"/>
@@ -9715,13 +9715,13 @@
       <c r="W147" s="4"/>
     </row>
     <row r="148" spans="1:25">
-      <c r="A148" s="197"/>
-      <c r="B148" s="193"/>
-      <c r="C148" s="194"/>
-      <c r="D148" s="195" t="s">
+      <c r="A148" s="163"/>
+      <c r="B148" s="159"/>
+      <c r="C148" s="160"/>
+      <c r="D148" s="161" t="s">
         <v>100</v>
       </c>
-      <c r="E148" s="197" t="s">
+      <c r="E148" s="163" t="s">
         <v>186</v>
       </c>
       <c r="F148" s="31"/>
@@ -9732,7 +9732,7 @@
       <c r="K148" s="49"/>
       <c r="L148" s="48"/>
       <c r="M148" s="48"/>
-      <c r="N148" s="170"/>
+      <c r="N148" s="231"/>
       <c r="O148" s="4"/>
       <c r="P148" s="5"/>
       <c r="Q148" s="4"/>
@@ -9744,13 +9744,13 @@
       <c r="W148" s="4"/>
     </row>
     <row r="149" spans="1:25" s="24" customFormat="1" ht="16" thickBot="1">
-      <c r="A149" s="236"/>
-      <c r="B149" s="235"/>
-      <c r="C149" s="227"/>
-      <c r="D149" s="256" t="s">
+      <c r="A149" s="202"/>
+      <c r="B149" s="201"/>
+      <c r="C149" s="193"/>
+      <c r="D149" s="220" t="s">
         <v>552</v>
       </c>
-      <c r="E149" s="236"/>
+      <c r="E149" s="202"/>
       <c r="F149" s="50" t="s">
         <v>336</v>
       </c>
@@ -9771,7 +9771,7 @@
       <c r="M149" s="72" t="s">
         <v>456</v>
       </c>
-      <c r="N149" s="171"/>
+      <c r="N149" s="232"/>
       <c r="O149" s="18"/>
       <c r="P149" s="17"/>
       <c r="Q149" s="18"/>
@@ -9810,68 +9810,68 @@
       <c r="Y151" s="11"/>
     </row>
     <row r="152" spans="1:25">
-      <c r="A152" s="197" t="s">
+      <c r="A152" s="163" t="s">
         <v>307</v>
       </c>
-      <c r="B152" s="193"/>
-      <c r="C152" s="257" t="s">
+      <c r="B152" s="159"/>
+      <c r="C152" s="229" t="s">
         <v>241</v>
       </c>
-      <c r="D152" s="195" t="s">
+      <c r="D152" s="161" t="s">
         <v>567</v>
       </c>
-      <c r="E152" s="197" t="s">
+      <c r="E152" s="163" t="s">
         <v>569</v>
       </c>
-      <c r="F152" s="193" t="s">
+      <c r="F152" s="159" t="s">
         <v>573</v>
       </c>
     </row>
     <row r="153" spans="1:25">
-      <c r="A153" s="197"/>
-      <c r="B153" s="193"/>
-      <c r="C153" s="257"/>
-      <c r="D153" s="195" t="s">
+      <c r="A153" s="163"/>
+      <c r="B153" s="159"/>
+      <c r="C153" s="229"/>
+      <c r="D153" s="161" t="s">
         <v>567</v>
       </c>
-      <c r="E153" s="197" t="s">
+      <c r="E153" s="163" t="s">
         <v>568</v>
       </c>
-      <c r="F153" s="195" t="s">
+      <c r="F153" s="161" t="s">
         <v>574</v>
       </c>
     </row>
     <row r="154" spans="1:25">
-      <c r="A154" s="197"/>
-      <c r="B154" s="193"/>
-      <c r="C154" s="257"/>
-      <c r="D154" s="195" t="s">
+      <c r="A154" s="163"/>
+      <c r="B154" s="159"/>
+      <c r="C154" s="229"/>
+      <c r="D154" s="161" t="s">
         <v>570</v>
       </c>
-      <c r="E154" s="197" t="s">
+      <c r="E154" s="163" t="s">
         <v>571</v>
       </c>
     </row>
     <row r="155" spans="1:25">
-      <c r="A155" s="197"/>
-      <c r="B155" s="193"/>
-      <c r="C155" s="257"/>
-      <c r="D155" s="198"/>
-      <c r="E155" s="258"/>
+      <c r="A155" s="163"/>
+      <c r="B155" s="159"/>
+      <c r="C155" s="229"/>
+      <c r="D155" s="164"/>
+      <c r="E155" s="221"/>
     </row>
     <row r="156" spans="1:25">
-      <c r="A156" s="197"/>
-      <c r="B156" s="193"/>
-      <c r="C156" s="257"/>
-      <c r="D156" s="195"/>
-      <c r="E156" s="258"/>
+      <c r="A156" s="163"/>
+      <c r="B156" s="159"/>
+      <c r="C156" s="229"/>
+      <c r="D156" s="161"/>
+      <c r="E156" s="221"/>
     </row>
     <row r="157" spans="1:25">
-      <c r="A157" s="197"/>
-      <c r="B157" s="193"/>
-      <c r="C157" s="257"/>
-      <c r="D157" s="195"/>
-      <c r="E157" s="197"/>
+      <c r="A157" s="163"/>
+      <c r="B157" s="159"/>
+      <c r="C157" s="229"/>
+      <c r="D157" s="161"/>
+      <c r="E157" s="163"/>
     </row>
     <row r="158" spans="1:25" s="22" customFormat="1" ht="7" customHeight="1">
       <c r="A158" s="19"/>
@@ -9896,6 +9896,12 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="N1:N2"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="K1:L1"/>
     <mergeCell ref="V3:W3"/>
     <mergeCell ref="R1:S2"/>
     <mergeCell ref="C152:C157"/>
@@ -9912,12 +9918,6 @@
     <mergeCell ref="B96:C96"/>
     <mergeCell ref="P1:Q2"/>
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="O1:O2"/>
-    <mergeCell ref="N1:N2"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="K1:L1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>